<commit_message>
Atualizacao dos codigos e artigos
Correções dos códigos em Python na sequencia de escape dos caminhos das pastas. Remoção de documentos de pesquisas de séries temporais, fora do escopo deste projeto
</commit_message>
<xml_diff>
--- a/Ontologia de Solos/Pesquisa SCOPUS/Pesquisa_Ontologia_Solos.xlsx
+++ b/Ontologia de Solos/Pesquisa SCOPUS/Pesquisa_Ontologia_Solos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EC4951-B171-4175-97D8-3AD0F8F9A947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B8A07F-77B0-41C8-9D79-778B378BC939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="131">
   <si>
     <t>ID do Documento</t>
   </si>
@@ -82,6 +82,9 @@
     <t>Kendig, Catherine</t>
   </si>
   <si>
+    <t>2024</t>
+  </si>
+  <si>
     <t>Journal of Social Ontology</t>
   </si>
   <si>
@@ -131,6 +134,9 @@
   </si>
   <si>
     <t>Abdullah, Azween; Murali, E.; Sreeji, S.; Balusamy, Balamurugan; Rajashree, S.</t>
+  </si>
+  <si>
+    <t>2023</t>
   </si>
   <si>
     <t>International Journal on Recent and Innovation Trends in Computing and Communication</t>
@@ -186,6 +192,9 @@
     <t>Mummigatti, Kushala Vijaya Kumar; Chandramouli, Supriya Maganahalli</t>
   </si>
   <si>
+    <t>2022</t>
+  </si>
+  <si>
     <t>Revue d'Intelligence Artificielle</t>
   </si>
   <si>
@@ -232,6 +241,9 @@
     <t>Krzywoszynska, Anna; Marchesi, Greta</t>
   </si>
   <si>
+    <t>2020</t>
+  </si>
+  <si>
     <t>Environmental Humanities</t>
   </si>
   <si>
@@ -285,6 +297,9 @@
     <t>Shu, Yanfeng; Liu, Qing</t>
   </si>
   <si>
+    <t>2015</t>
+  </si>
+  <si>
     <t>Proceedings - 21st International Congress on Modelling and Simulation, MODSIM 2015</t>
   </si>
   <si>
@@ -321,6 +336,9 @@
     <t>Das, Manoranjan; Malhotra, P.K.; Marwaha, Sudeep; Pandey, R.N.</t>
   </si>
   <si>
+    <t>2014</t>
+  </si>
+  <si>
     <t>Indian Journal of Agricultural Sciences</t>
   </si>
   <si>
@@ -330,44 +348,77 @@
     <t>United States Department of Agriculture (USDA) Soil Taxonomy is based on soil properties that can be objectively observed and measured in the natural conditions as they exist today. There are many soil classification systems but USDA Soil Taxonomy is most accepted worldwide. Ontologies are the new form of knowledge representation that acts in synergy with agents and Semantic Web Architecture. Soil ontology developed for USDA soil taxonomy has been used to develop a query interface that will help in detailed study of soil taxonomy, classification of new soil as well as exchange knowledge between software agents and systems. This is a web based application having N-tier architecture. Application development environment is NetBeans 6. 9 editor and Protégé. Web development technology is Java Server Pages (JSP). Programming languages JAVA and SPARQL are used for querying. Client interface is developed with Hyper Text Markup Language (HTML), Cascading Style Sheet (CSS) and JavaScript. Third tier of software consist of database which is in MS-SQL server 2005. Other two layers are Web Ontology Language (OWL) Ontology layer and Semantic Web Framework layer. OWL layer contains soil taxonomy information in the form of Ontology. Semantic Web Framework layer is implemented using JENA. In the search panel user can search anything related to USDA Soil Taxonomy, which comprises of twelve orders. However, this software contains information about seven soil orders reported in India. Domain experts can see and edit the knowledge base (i. e. Soil Ontology) or can suggest anything related to the creation of Soil Taxonomy Ontology through WebProtégé.</t>
   </si>
   <si>
-    <t>MFAMAD</t>
-  </si>
-  <si>
-    <t>MFAM-AD: an anomaly detection model for multivariate time series using attention mechanism to fuse multi-scale features</t>
-  </si>
-  <si>
-    <t>Xia, Shengjie; Sun, Wu; Zou, Xiaofeng; Chen, Panfeng; Ma, Dan; Xu, Huarong; Chen, Mei; Li, Hui</t>
-  </si>
-  <si>
-    <t>PeerJ Computer Science</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.7717/PEERJ-CS.2201</t>
-  </si>
-  <si>
-    <t>"time series" and gecco"</t>
-  </si>
-  <si>
-    <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\MFAMAD.txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Este documento apresenta o MFAM-AD, um novo modelo para detecção de anomalias em séries temporais multivariadas, que combina redes neurais convolucionais (CNNs) e redes de memória de longo prazo bidirecionais (Bi-LSTMs). O modelo utiliza camadas convolucionais paralelas com um mecanismo de atenção para extrair e fundir características em múltiplas escalas, enquanto as Bi-LSTMs capturam dependências temporais para reconstruir a série temporal e detectar anomalias baseadas em erros de reconstrução. Os resultados experimentais em conjuntos de dados públicos demonstram que o MFAM-AD supera vários modelos de linha de base e em alguns conjuntos de dados, supera até mesmo o modelo de última geração DCdetector, validando sua eficácia na detecção de anomalias. O MFAM-AD oferece uma solução robusta e eficaz para detecção de anomalias em séries temporais multivariadas, com potencial para diversas aplicações no mundo real.
+    <t>maconto</t>
+  </si>
+  <si>
+    <t>MaCOnto: A robust maize crop ontology based on soils, fertilizers and irrigation knowledge</t>
+  </si>
+  <si>
+    <t>Aminu, Enesi Femi; Oyefolahan, Ishaq Oyebisi; Abdullahi, Muhammad Bashir; Salaudeen, Muhammadu Tajudeen</t>
+  </si>
+  <si>
+    <t>Intelligent Systems with Applications</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.iswa.2022.200125</t>
+  </si>
+  <si>
+    <t>"soil knowledge" limit "science computer"</t>
+  </si>
+  <si>
+    <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\maconto.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O artigo apresenta o MaCOnto, uma ontologia robusta para o domínio do milho, focada em solos, fertilizantes e irrigação, construída com OWL e regras SWRL.  A ontologia usa uma metodologia de engenharia de ontologia em seis etapas, incluindo a evolução autônoma por meio do WordNet. O MaCOnto foi validado com sucesso por especialistas em domínio através de 80 questões de competência modeladas em lógica de primeira ordem e implementadas como regras, demonstrando capacidades de inferência. A avaliação estrutural baseada em oito métricas demonstra um desempenho superior em comparação com ontologias OWL existentes, confirmando sua robustez.
 </t>
   </si>
   <si>
-    <t>Multivariate time series anomaly detection has garnered significant attention in fields such as IT operations, finance, medicine, and industry. However, a key challenge lies in the fact that anomaly patterns often exhibit multi-scale temporal variations, which existing detection models often fail to capture effectively. This limitation significantly impacts detection accuracy. To address this issue, we propose the MFAM-AD model, which combines the strengths of convolutional neural networks (CNNs) and bidirectional long short-term memory (Bi-LSTM). The MFAM-AD model is designed to enhance anomaly detection accuracy by seamlessly integrating temporal dependencies and multi-scale spatial features. Specifically, it utilizes parallel convolutional layers to extract features across different scales, employing an attention mechanism for optimal feature fusion. Additionally, Bi-LSTM is leveraged to capture time-dependent information, reconstruct the time series and enable accurate anomaly detection based on reconstruction errors. In contrast to existing algorithms that struggle with inadequate feature fusion or are confined to single-scale feature analysis, MFAMAD effectively addresses the unique challenges of multivariate time series anomaly detection. Experimental results on five publicly available datasets demonstrate the superiority of the proposed model. Specifically, on the datasets SMAP, MSL, and SMD1-1, our MFAM-AD model has the second-highest F1 score after the current state-of-the-art DCdetector model. On the datasets NIPS-TS-SWAN and NIPS-TS-GECCO, the F1 scores of MAFM-AD are 0.046 (6.2%) and 0.09 (21.3%) higher than those of DCdetector, respectively(the value ranges from 0 to 1). These findings validate the MFAMAD model’s efficacy in multivariate time series anomaly detection, highlighting its potential in various real-world applications. © 2024 Xia et al.</t>
-  </si>
-  <si>
-    <t>"soil knowledge" limit "science computer"</t>
-  </si>
-  <si>
-    <t>maconto</t>
+    <t>The demand for relevant information in a timely manner portrays the significance of knowledge management in all areas of lives; for instance, agriculture. To this end, soils, fertilizers and irrigation as agronomic concepts are essential knowledge inputs for any crops, such as maize. Conversely, there is always difficulty in timely retrieval of these relevant information owing to the unstructured nature of data in repositories, and complexity of concepts mismatch. Sequel to this development, ontology, a semantic data modeling technique is promising as it has been recently employed to deal with these challenges across different domains. However, the robustness of ontology, in terms of semantic expressivity of hidden knowledge, and autonomous growth of ontology leave some gaps to contend with. In view of this development, this research aims to design a robust OWL Rule based ontology for maize crop domain by considering primarily soils, fertilizers and irrigation agronomic concepts capable to evolve autonomously. The proposed ontology herein christened MaCOnto, is developed using the adapted six steps ontology-engineering principle. Over 1,430 entities are encoded in OWL; eighty Competency Questions (CQs) validated by domain experts are modeled in FOL, and implemented as rules via SWRL. Thus, the ontology is queried by SQWRL. Besides, the novel algorithmic design for the ontology to autonomously evolve is implemented in Java environment by employing WordNet. The results obtained from structural based evaluation show an outstanding performance across the eight metrics. Similarly, the results of the competency-based evaluation are also promising. Therefore, the proposed MaCOnto is a robust application based ontology capable to infer and responds to user's query based on its contextual information. © 2022</t>
   </si>
   <si>
     <t>Causal_Research_on_Soil</t>
   </si>
   <si>
+    <t>Causal Research on Soil Temperature and Moisture Content at Different Depths</t>
+  </si>
+  <si>
+    <t>Cao, Zhihao; Mu, Shaomin; Xu, Li; Shao, Mingfeng; Qu, Hongchun</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>IEEE Access</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1109/ACCESS.2021.3064264</t>
+  </si>
+  <si>
+    <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Causal_Research_on_Soil.txt</t>
+  </si>
+  <si>
+    <t>Este documento investiga as relações causais entre a temperatura e o teor de umidade do solo em diferentes profundidades, usando modelagem empírica dinâmica (EDM). O estudo demonstra que a complexidade e as relações de causa e efeito no sistema solo variam entre o verão e o inverno. Através do algoritmo de projeção simples e do algoritmo de mapeamento cruzado convergente (CCM), os autores identificam que a transferência de energia térmica entre as camadas do solo e a atividade da água influenciam significativamente as relações causais. Os resultados obtidos são consistentes com o ambiente real do solo e fornecem uma nova perspectiva para a pesquisa da dinâmica do solo.</t>
+  </si>
+  <si>
+    <t>The soil system is complex and dynamic, making it difficult to understand using traditional statistical approaches. In this paper, we analyze the causal relationship of soil temperature and moisture content at different depths in summer and winter based on dynamic empirical modelling. Specifically, we describe the complexity of soil temperature and moisture content system through mathematical methods. Moreover, we demonstrate the direction and magnitude of causal relationship between soil moisture content and temperature at different depths by equation-free methods. Besides, we describe the difference of soil system properties in summer and winter through causal research. The experiments show that results obtained are consistent with the actual soil environment. The causality is described by dynamic empirical modelling rather than prior soil knowledge. The paper may provide a new idea for soil dynamics research.  © 2013 IEEE.</t>
+  </si>
+  <si>
     <t>Temporal-space-variation</t>
+  </si>
+  <si>
+    <t>Temporal-spatial variations monitoring of soil moisture using microwave polarization difference index</t>
+  </si>
+  <si>
+    <t>Duan, Si-Bo; Li, Zhao-Liang; Tang, Ronglin; Tang, Bo-Hui; Wu, Hua; Jiang, Xiaoguang</t>
+  </si>
+  <si>
+    <t>International Geoscience and Remote Sensing Symposium (IGARSS)</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1109/IGARSS.2014.6947183</t>
+  </si>
+  <si>
+    <t>Soil moisture is a key variable that influences the redistribution of the radiant energy and the runoff generation and percolation of water in soil. Knowledge of soil moisture temporal-spatial variations is important in a wide range of studies. This study aims to investigate the temporal-spatial variations of soil moisture using microwave polarization difference index (MPDI). The AMSR-E/Aqua Daily Global Quarter-Degree Gridded Brightness Temperature at 10.65 GHz channel was used to calculate the MPDI. In addition, the AMSR-E/Aqua Daily L3 Surface Soil Moisture was used in this study. The temporal and spatial patterns between the MPDI and soil moisture were analyzed. The results indicate that the temporal and spatial patterns of the MPDI are consistent with those of soil moisture. The MPDI reflects the temporal and spatial variations of soil moisture. © 2014 IEEE.</t>
   </si>
 </sst>
 </file>
@@ -730,15 +781,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" activeCellId="1" sqref="G16 H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="7" max="7" width="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -804,414 +856,448 @@
       <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="D2">
-        <v>2024</v>
+      <c r="D2" t="s">
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3">
-        <v>2024</v>
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" t="s">
         <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4">
-        <v>2023</v>
-      </c>
-      <c r="E4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" t="s">
-        <v>41</v>
-      </c>
-      <c r="N4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5">
-        <v>2023</v>
-      </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J5" t="s">
-        <v>41</v>
-      </c>
       <c r="N5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6">
-        <v>2022</v>
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J6" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="N6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="Q6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7">
-        <v>2022</v>
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8">
-        <v>2020</v>
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I8" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="J8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N8" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="Q8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D9">
         <v>2015</v>
       </c>
       <c r="E9" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="J9" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="N9" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="Q9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10">
-        <v>2015</v>
+        <v>89</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N10" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" t="s">
         <v>90</v>
       </c>
-      <c r="C11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11">
-        <v>2015</v>
-      </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N11" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12">
-        <v>2014</v>
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
       </c>
       <c r="E12" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="F12" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="G12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N12" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C13" t="s">
-        <v>103</v>
-      </c>
-      <c r="D13">
-        <v>2024</v>
+        <v>109</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F13" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="G13" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="H13" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="I13" t="s">
-        <v>108</v>
-      </c>
-      <c r="J13" t="s">
-        <v>31</v>
+        <v>114</v>
       </c>
       <c r="N13" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="Q13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>116</v>
+      </c>
+      <c r="B14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" t="s">
+        <v>121</v>
       </c>
       <c r="G14" t="s">
-        <v>110</v>
+        <v>112</v>
+      </c>
+      <c r="H14" t="s">
+        <v>122</v>
+      </c>
+      <c r="I14" t="s">
+        <v>123</v>
+      </c>
+      <c r="N14" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" t="s">
+        <v>129</v>
+      </c>
+      <c r="G15" t="s">
         <v>112</v>
       </c>
-      <c r="G15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>113</v>
-      </c>
-      <c r="G16" t="s">
-        <v>110</v>
+      <c r="N15" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nova atualização e bibliografia
</commit_message>
<xml_diff>
--- a/Ontologia de Solos/Pesquisa SCOPUS/Pesquisa_Ontologia_Solos.xlsx
+++ b/Ontologia de Solos/Pesquisa SCOPUS/Pesquisa_Ontologia_Solos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q294"/>
+  <dimension ref="A1:Q324"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20479,11 +20479,31 @@
           <t>the-role-of-soils-in-learning-and-inspiration-physical-and-psychological-experiences-and-in-supporting</t>
         </is>
       </c>
-      <c r="B292" t="inlineStr"/>
-      <c r="C292" t="inlineStr"/>
-      <c r="D292" t="inlineStr"/>
-      <c r="E292" t="inlineStr"/>
-      <c r="F292" t="inlineStr"/>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>The role of soils in learning and inspiration, physical and psychological experiences, and in supporting identities</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>McElwee, Pamela</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>Philosophical Transactions of the Royal Society B: Biological Sciences</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1098/rstb.2020.0184</t>
+        </is>
+      </c>
       <c r="G292" t="inlineStr">
         <is>
           <t>snowballing Making-time-for-soil</t>
@@ -20498,8 +20518,16 @@
       <c r="J292" t="inlineStr"/>
       <c r="K292" t="inlineStr"/>
       <c r="L292" t="inlineStr"/>
-      <c r="M292" t="inlineStr"/>
-      <c r="N292" t="inlineStr"/>
+      <c r="M292" t="inlineStr">
+        <is>
+          <t>Art; Conservation of Natural Resources; Cultural Characteristics; Environment; Gardening; Humans; Recreation; Religion; Social Justice; Soil; anthropogenic effect; social justice; soil analysis; soil ecosystem; art; cultural factor; environment; environmental protection; gardening; human; psychology; recreation; religion; social justice; soil</t>
+        </is>
+      </c>
+      <c r="N292" t="inlineStr">
+        <is>
+          <t>This paper reviews the literature on soil and nature's contributions to people (NCP) around learning and inspiration, physical and psychological experiences, and supporting identities, revealing a range of relationships to imagining, understanding and experiencing soil. Often labelled elsewhere as 'cultural ecosystem services', these NCP provide a range of benefits that are mostly non-material, non-consumptive and intangible. The review finds that NCP framings help to highlight how soils have contributed to inspiring learning and creative works, like art; to mental and physical health benefits, such as through recreation and gardening; and to cultural identities and practices, including religious practices and efforts for social justice. Overall, soils have played a large role in human creative endeavours, are the root of significant relationships to the environment and can be conceptualized through key metaphors, ideas and theory as a bridge linking culture and nature together. Yet despite the wide-ranging contributions of soils to these NCP, the literature remains uneven and much more remains to be understood, including how relational values of care and stewardship with soils can be fostered and how attention to the co-produced 'biosocial' nature of soil can help improve practices for soil health. This article is part of the theme issue 'The role of soils in delivering Nature's Contributions to People'. © 2021 The Author(s).</t>
+        </is>
+      </c>
       <c r="O292" t="inlineStr"/>
       <c r="P292" t="inlineStr"/>
       <c r="Q292" t="inlineStr">
@@ -20514,11 +20542,31 @@
           <t>emplaced-care-and-atmospheric-politics-in-unbreathable-worlds</t>
         </is>
       </c>
-      <c r="B293" t="inlineStr"/>
-      <c r="C293" t="inlineStr"/>
-      <c r="D293" t="inlineStr"/>
-      <c r="E293" t="inlineStr"/>
-      <c r="F293" t="inlineStr"/>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>Emplaced care and atmospheric politics in unbreathable worlds</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>Kenner, Alison</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>Environment and Planning C: Politics and Space</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1177/2399654419851347</t>
+        </is>
+      </c>
       <c r="G293" t="inlineStr">
         <is>
           <t>snowballing Making-time-for-soil</t>
@@ -20533,8 +20581,16 @@
       <c r="J293" t="inlineStr"/>
       <c r="K293" t="inlineStr"/>
       <c r="L293" t="inlineStr"/>
-      <c r="M293" t="inlineStr"/>
-      <c r="N293" t="inlineStr"/>
+      <c r="M293" t="inlineStr">
+        <is>
+          <t>United States; asthma; environmental politics; pathology; theoretical study</t>
+        </is>
+      </c>
+      <c r="N293" t="inlineStr">
+        <is>
+          <t>This paper contributes to emerging theories of unbreathable space by showing how breathers with asthma engage environments and atmospheres as the substrate of their everyday lives. Drawing on in-depth interviews with more than 80 asthma sufferers living in the United States, I show how nonpharmaceutical care practices are used to breathe in place. First, I argue that attunement operates as a labor of care that engages with and creates the substrate of everyday life. Next, I describe a range of emplacement tactics that breathers use to navigate atmospheres and environments that are potentially risky, or that immediately produce asthma symptoms. Emplaced care involves situating oneself in ways that protect the breathing body within the sociomaterial spaces of everyday life. Finally, people with asthma are orientated differently than other breathers who may share the same atmosphere, but are not pathologically sensitized to it. These narratives of asthma care lend insight into emergent atmospheric politics by showing how differently attuned breathers care through environments by isolating, distancing, and barricading themselves from the world and others. © The Author(s) 2019.</t>
+        </is>
+      </c>
       <c r="O293" t="inlineStr"/>
       <c r="P293" t="inlineStr"/>
       <c r="Q293" t="inlineStr">
@@ -20549,11 +20605,31 @@
           <t>Microbial-antagonism-in-the-trentino-alps-negotiating-spacetimes-and-ownership</t>
         </is>
       </c>
-      <c r="B294" t="inlineStr"/>
-      <c r="C294" t="inlineStr"/>
-      <c r="D294" t="inlineStr"/>
-      <c r="E294" t="inlineStr"/>
-      <c r="F294" t="inlineStr"/>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>Microbial antagonism in the trentino alps negotiating spacetimes and ownership through the production of raw milk cheese in alpine high mountain summer pastures</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Raffaetà, Roberta</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>Current Anthropology</t>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1086/714348</t>
+        </is>
+      </c>
       <c r="G294" t="inlineStr">
         <is>
           <t>snowballing Making-time-for-soil</t>
@@ -20569,7 +20645,11 @@
       <c r="K294" t="inlineStr"/>
       <c r="L294" t="inlineStr"/>
       <c r="M294" t="inlineStr"/>
-      <c r="N294" t="inlineStr"/>
+      <c r="N294" t="inlineStr">
+        <is>
+          <t>In this paper I analyze fermentation practices in the production of cheese in Alpine high mountain summer pastures and their connection to politics of space, heritage, and ownership in times of ecological, social, scientific, and economic transition. In the Trentino Alps, fermentation is a technology for enacting different spacetimes in that it is not only a technical act but is also connected to how people practice and give meaning to places. I will focus on how fermentation participates in the composition of different human, more-than-human, and microbial spacetimes, which I call “utopias,” “heterotopias,” and “atopias.” In these spacetimes, fermentation translates space into cheese through different logics: overlap, transduction, or abstraction. Discussing how fermentation is managed and perceived gives us the opportunity to reflect on who owns the Alps and leads to a debate on how to constitute sustainable and just futures. Fermentation plays a key role in scientific innovation as well as in social innovation as to how the Alps will be assigned value and ownership. © 2021 The Wenner-Gren Foundation for Anthropological Research. All rights reserved.</t>
+        </is>
+      </c>
       <c r="O294" t="inlineStr"/>
       <c r="P294" t="inlineStr"/>
       <c r="Q294" t="inlineStr">
@@ -20577,6 +20657,1600 @@
           <t>Sim</t>
         </is>
       </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>Attending-to-nature-Understanding-care-and-caring-relations</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>Attending to nature: Understanding care and caring relations in forest management in the UK</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>O'Flynn, Trish; Geoghegan, Hilary; Dyke, Alison; de Bruin, Annemarieke</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>Journal of Rural Studies</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.jrurstud.2021.05.022</t>
+        </is>
+      </c>
+      <c r="G295" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H295" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Attending-to-nature-Understanding-care-and-caring-relations.txt</t>
+        </is>
+      </c>
+      <c r="I295" t="inlineStr"/>
+      <c r="J295" t="inlineStr"/>
+      <c r="K295" t="inlineStr"/>
+      <c r="L295" t="inlineStr"/>
+      <c r="M295" t="inlineStr">
+        <is>
+          <t>United Kingdom; conservation; decision making; environmental values; forest management; forestry practice; nature-society relations; participatory approach; public space; rural area; tree</t>
+        </is>
+      </c>
+      <c r="N295" t="inlineStr">
+        <is>
+          <t>Increasing threats from pests and diseases fundamentally question what forest management is and must do in the 21st century. The sociological concept of ‘care’ offers new understandings of forest management as intimate and emotional relationships between people and trees. In this paper, we examine the empirical realities of conservation forest management at a UK publicly owned site to reveal the social, economic, and institutional contexts of care and caring relations and their role in management decisions. This in-depth qualitative case study uses walking interviews with staff from all levels of the organisation and participatory data testing to show how care underpins the work of forest management, that forests are made and sustained through caring practices, and that management decisions are influenced by caring relations. Through the care framework we highlight the complexities of real-life decision-making and offer implications for forestry policy and practice. Applying the well-established components of care in a new setting, wherein the caring relations involve nonhumans, we extend care theory and demonstrate the potential of the single case study for deeply contextual forest and conservation research. © 2021 Elsevier Ltd</t>
+        </is>
+      </c>
+      <c r="O295" t="inlineStr"/>
+      <c r="P295" t="inlineStr"/>
+      <c r="Q295" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>Metagenomics-approaches-in-microbial-ecology</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>Metagenomics approaches in microbial ecology and research for sustainable agriculture; [Metagenomische Ansätze in der mikrobiellen Ökologie und Forschung für nachhaltige Landwirtschaft]</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>Meunier, Robert; Bayır, Saliha</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>Zeitschrift fur Technikfolgenabschatzung in Theorie und Praxis / Journal for Technology Assessment in Theory and Practice</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.14512/tatup.30.2.24</t>
+        </is>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H296" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Metagenomics-approaches-in-microbial-ecology.txt</t>
+        </is>
+      </c>
+      <c r="I296" t="inlineStr"/>
+      <c r="J296" t="inlineStr"/>
+      <c r="K296" t="inlineStr"/>
+      <c r="L296" t="inlineStr"/>
+      <c r="M296" t="inlineStr"/>
+      <c r="N296" t="inlineStr">
+        <is>
+          <t>• Technologies such as next generation sequencing (NGS) are transforming research fields at the methodological, conceptual, and or-ganizational level. They open up new possibilities and bring with them new commitments and inherent limitations. We show from a philosophy of science perspective how NGS-based metagenomics has trans-formed microbial ecology and, with it, parts of agricultural soil science, which integrate ecological approaches with the aim to inform agricultural practices. We reconstruct agricultural science as design science (sensu Niiniluoto) and describe how the possibilities, commitments, and limitations of metagenomics approaches in microbial ecology shape values, situation assessments, and recommendations for inter-ventions of soil microbiology in the context of sustainable agriculture. © 2021, Oekom Verlag. All rights reserved.</t>
+        </is>
+      </c>
+      <c r="O296" t="inlineStr"/>
+      <c r="P296" t="inlineStr"/>
+      <c r="Q296" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>Words-Are-Essential-but-Underexamined-Research-Tools-for-Microbes-and-Microbiomes</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>Words Are Essential, but Underexamined, Research Tools for Microbes and Microbiomes</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>Szymanski, Erika</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>mSystems</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1128/mySystems.00769-21</t>
+        </is>
+      </c>
+      <c r="G297" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H297" t="inlineStr"/>
+      <c r="I297" t="inlineStr"/>
+      <c r="J297" t="inlineStr"/>
+      <c r="K297" t="inlineStr"/>
+      <c r="L297" t="inlineStr"/>
+      <c r="M297" t="inlineStr">
+        <is>
+          <t>analogical reasoning; attention; expectation; human; human experiment; language; literature; microbiome; microorganism; nonhuman; review; synthetic biology; thinking; yeast</t>
+        </is>
+      </c>
+      <c r="N297" t="inlineStr">
+        <is>
+          <t>Language constitutes an essential set of scientific construction tools, not only for communicating knowledge, but for conceptualizing the world. Metaphors in particular, as conventions that guide and reproduce analogical reasoning, merit attention that they largely do not receive. My research addresses this deficit by examining how metaphors for handling microbes shape possibilities for working with yeast and bacteria in synthetic biology, microbiome research, and other fields that reconfigure what microbes can be. Though poised to reexamine assumptions, these fields routinely rest on metaphors and other language tools that quietly embed ways of thinking that may work against wider aims-for example, imagining bacteria as imperfect machines that should therefore be rendered increasingly passive and controllable. Researchers, therefore, need to examine how language tools structure their observations and expectations so that the tools they choose are appropriate for the work they want to do. © 2021 Szymanski.</t>
+        </is>
+      </c>
+      <c r="O297" t="inlineStr"/>
+      <c r="P297" t="inlineStr"/>
+      <c r="Q297" t="inlineStr"/>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>no-future-for-care-without-new-digital-media-making-time(s)-for-mediated-informal-care-practices</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>No future for care without new digital media? Making time(s) for mediated informal care practices in later life</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>López-Gómez, Daniel; Beneito-Montagut, Roser; García-Santesmases, Andrea</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>International Journal of Cultural Studies</t>
+        </is>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1177/1367877920951818</t>
+        </is>
+      </c>
+      <c r="G298" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H298" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\no-future-for-care-without-new-digital-media-making-time(s)-for-mediated-informal-care-practices.txt</t>
+        </is>
+      </c>
+      <c r="I298" t="inlineStr"/>
+      <c r="J298" t="inlineStr"/>
+      <c r="K298" t="inlineStr"/>
+      <c r="L298" t="inlineStr"/>
+      <c r="M298" t="inlineStr"/>
+      <c r="N298" t="inlineStr">
+        <is>
+          <t>There is a growing interest in using social media and digital platforms as allies to strengthen social support among the aged. Drawing on ethnographic interviews and observations of 21 people in their 80s, the article foregrounds the multiple and intersecting temporalities of informal mediated care practices in later life through an exploration of the wide range of infrastructures on which they rely, from social media platforms to housing and urban infrastructure. We identify four temporalities of mediated informal care to assert the need to problematize the future-oriented temporalities of new caring media. The article paves the way to consider infrastructures of informal care as making time in multiple forms, irrespective of their newness or oldness, or the futures that every new piece of technology and service may potentially bring to our present. © The Author(s) 2020.</t>
+        </is>
+      </c>
+      <c r="O298" t="inlineStr"/>
+      <c r="P298" t="inlineStr"/>
+      <c r="Q298" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>towards-a-more-than-human-political-ecology-of-coastal-protection-coast-care-practices-in-aotearoa-new</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>Towards a more-than-human political ecology of coastal protection: Coast Care practices in Aotearoa New Zealand</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>Gesing, Friederike</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>Environment and Planning E: Nature and Space</t>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1177/2514848619860751</t>
+        </is>
+      </c>
+      <c r="G299" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H299" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\towards-a-more-than-human-political-ecology-of-coastal-protection-coast-care-practices-in-aotearoa-new.txt</t>
+        </is>
+      </c>
+      <c r="I299" t="inlineStr"/>
+      <c r="J299" t="inlineStr"/>
+      <c r="K299" t="inlineStr"/>
+      <c r="L299" t="inlineStr"/>
+      <c r="M299" t="inlineStr"/>
+      <c r="N299" t="inlineStr">
+        <is>
+          <t>Coastal protection measures are intended to stabilize the boundaries of land and sea—and of private property. But structural engineering solutions, such as seawalls, have negative side-effects in terms of environmental and climate justice: they cause erosion of adjacent areas, they limit public access, and they can lead to the loss of sandy beaches. So-called “soft” coastal protection approaches promise more sustainable and just alternatives. The article explores the role of the more-than-human in such practices. Arguing that the popular framing of coastal protection as “working with nature” is a strategic naturalization, the paper aims to develop a more-than-human take on the political ecology of coastal protection. The empirical basis is built from ethnographic material on volunteer dune restoration by Coast Care groups in Aotearoa New Zealand. The analysis shows that the “multispecies agencies” (Locke, 2013) at work in various practices associated with Coast Care include communities of plants and animals, human care work and artefacts, as well as abiotic elements such as sand, wind, water and concrete. The article argues that to foster political and practical engagements for more sustainable coastal naturecultures, these entanglements should be made explicit and accountable. A more-than-human political ecology approach to understand the promises of soft coastal protection therefore combines three analytic sensibilities. Firstly, it looks at the ontological politics and categorization practices that define and enact specific versions of coastal nature. Secondly, it focuses on the politics of care in multispecies worlds, including the abiotic. And thirdly, it takes into account the “ordinary politics” of contested coastal space, decision-making and planning. © The Author(s) 2019.</t>
+        </is>
+      </c>
+      <c r="O299" t="inlineStr"/>
+      <c r="P299" t="inlineStr"/>
+      <c r="Q299" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>Entangled-materialities-Caring-for-soil-communities-at-glass-industry-sites</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>Entangled materialities: Caring for soil communities at glass industry sites</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Latva-Somppi, Riikka; Mäkelä, Maarit; Lindström, Kristina; Ståhl, Åsa</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>FormAkademisk</t>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.7577/FORMAKADEMISK.4180</t>
+        </is>
+      </c>
+      <c r="G300" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H300" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Entangled-materialities-Caring-for-soil-communities-at-glass-industry-sites.txt</t>
+        </is>
+      </c>
+      <c r="I300" t="inlineStr"/>
+      <c r="J300" t="inlineStr"/>
+      <c r="K300" t="inlineStr"/>
+      <c r="L300" t="inlineStr"/>
+      <c r="M300" t="inlineStr"/>
+      <c r="N300" t="inlineStr">
+        <is>
+          <t>This paper discusses craft and design practices through their impact on the environment. We consider how to act concerning the consequences of the craft and design industry. Also, we reflect on the agency of our field of practice in changing how we perceive the environment. We present three case studies of the European glass industry sites in Sweden, Italy and Finland, where we study contamination of the soil with participatory, speculative and craft methods. Through these cases, we reflect on our role in soil communities and ask how we may act in them with responsibility, hope and care. We conclude by proposing to act locally, to share our practices and make them visible, expanding our situated, personal skills and knowledge towards the political. © 2021, The Assosiation FormAkademisk. All rights reserved.</t>
+        </is>
+      </c>
+      <c r="O300" t="inlineStr"/>
+      <c r="P300" t="inlineStr"/>
+      <c r="Q300" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>Calling-for-a-Plurality-of-Perspectives-on-Design-Futuring-An-Un-Manifesto</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>Calling for a Plurality of Perspectives on Design Futuring: An Un-Manifesto</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>Howell, Noura; Schulte, Britta F.; Twigger Holroyd, Amy; Fatás Arana, Rocío; Sharma, Sumita; Eden, Grace</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr">
+        <is>
+          <t>Conference on Human Factors in Computing Systems - Proceedings</t>
+        </is>
+      </c>
+      <c r="F301" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1145/3411763.3450364</t>
+        </is>
+      </c>
+      <c r="G301" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H301" t="inlineStr"/>
+      <c r="I301" t="inlineStr"/>
+      <c r="J301" t="inlineStr"/>
+      <c r="K301" t="inlineStr"/>
+      <c r="L301" t="inlineStr"/>
+      <c r="M301" t="inlineStr">
+        <is>
+          <t>Software engineering; Professional backgrounds; Singular points; Technological progress; Human engineering</t>
+        </is>
+      </c>
+      <c r="N301" t="inlineStr">
+        <is>
+          <t>The Futures Cone, a prominent model in design futuring, is useful for promoting discussions about possible, plausible, probable, and preferable futures. Yet this model has limitations, such as representing diverse human experiences as a singular point of "the present"and implicitly embedding notions of linear progress. Responding to this, we argue that a plurality of perspectives is needed to engage imaginations that depict a diverse unfolding of potential futures. Through reflecting on our own cultural and professional backgrounds, we offer five perspectives for design futuring as a contribution to this plurality: Parallel Presents, "I Am Time", Epithelial Metaphors, the Uncertainties Cone, and Meet (with) "Speculation". These perspectives open alternative approaches to design futuring, move outside prevalent notions of technological progress, and foreground interdependent, relational agencies. © 2021 Owner/Author.</t>
+        </is>
+      </c>
+      <c r="O301" t="inlineStr"/>
+      <c r="P301" t="inlineStr"/>
+      <c r="Q301" t="inlineStr"/>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>Algorithmic-food-justice-Co-designing-more-than-human-blockchain-futures-for-the-food-commons</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Algorithmic food justice: Co-designing more-than-human blockchain futures for the food commons</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Heitlinger, Sara; Houston, Lara</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr">
+        <is>
+          <t>Conference on Human Factors in Computing Systems - Proceedings</t>
+        </is>
+      </c>
+      <c r="F302" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1145/3411764.3445655</t>
+        </is>
+      </c>
+      <c r="G302" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H302" t="inlineStr"/>
+      <c r="I302" t="inlineStr"/>
+      <c r="J302" t="inlineStr"/>
+      <c r="K302" t="inlineStr"/>
+      <c r="L302" t="inlineStr"/>
+      <c r="M302" t="inlineStr">
+        <is>
+          <t>Agricultural robots; Blockchain; Financial markets; Human engineering; Co-designing; Co-designs; Economic values; Food system; Human values; Multi-species; Role play; Social and environmental; Fintech</t>
+        </is>
+      </c>
+      <c r="N302" t="inlineStr">
+        <is>
+          <t>The relationships that constitute the global industrial food system tend towards two dominant values that are creating unsustainable social and environmental inequalities. The frst is a human-centered perspective on food that privileges humans over all other species. The second is a view of food as a commodity to be traded for maximum economic value, rewarding a small number of shareholders. We present work that explores the unique algorithmic afordances of blockchain to create new types of value exchange and governance in the food system. We describe a project that used roleplay with urban agricultural communities to co-design blockchain-based food futures and explore the conditions for creating a thriving multispecies food commons.We discuss how the project helped rethink algorithmic food justice by reconfguring more-than-human values and reconfguring food as more-than-human commons. We also discuss some of the challenges and tensions arising from these explorations. © 2021 ACM.</t>
+        </is>
+      </c>
+      <c r="O302" t="inlineStr"/>
+      <c r="P302" t="inlineStr"/>
+      <c r="Q302" t="inlineStr"/>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>Human-nature-relations-in-urban-gardens-Explorations-with-camera-traps</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Human-nature relations in urban gardens: Explorations with camera traps</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>Vella, Kellie; Ploderer, Bernd; Brereton, Margot</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr">
+        <is>
+          <t>Conference on Human Factors in Computing Systems - Proceedings</t>
+        </is>
+      </c>
+      <c r="F303" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1145/3411764.3445438</t>
+        </is>
+      </c>
+      <c r="G303" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H303" t="inlineStr"/>
+      <c r="I303" t="inlineStr"/>
+      <c r="J303" t="inlineStr"/>
+      <c r="K303" t="inlineStr"/>
+      <c r="L303" t="inlineStr"/>
+      <c r="M303" t="inlineStr">
+        <is>
+          <t>Biodiversity; Conservation; Human engineering; Green spaces; Human nature; Natural sensing; Sensing technology; Urban biodiversity; Urban garden; Cameras</t>
+        </is>
+      </c>
+      <c r="N303" t="inlineStr">
+        <is>
+          <t>As cities grow, their people become increasingly distanced from nature except within private and public green spaces. Sensing technologies provide a means to harness curiosity about the animals living in these spaces, and possibly also connect interest to care. Yet little is known as to how people may use these technologies, or the implications for human-nature relations. To learn more, we gave commercial camera traps to ten adult participants to understand how they explored their gardens, what they wanted to learn, and what they did with this knowledge. We discovered trade-ofs between control and care; the usefulness of diferent media and mystery; the temporalities of engaging in natural sensing practice; and a prevalence of sharing media within households. We discuss design for convivial cohabitation with the creatures in our garden. This research contributes to better human-nature relations through citizen sensing, as well as HCI for urban biodiversity conservation. © 2021 ACM.</t>
+        </is>
+      </c>
+      <c r="O303" t="inlineStr"/>
+      <c r="P303" t="inlineStr"/>
+      <c r="Q303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>Trans-Temporal-pigs-Humans-spirits-and-the-temporal-multiplicity-of-pigs-in-Ifugao-the-Philippines</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr"/>
+      <c r="C304" t="inlineStr"/>
+      <c r="D304" t="inlineStr"/>
+      <c r="E304" t="inlineStr"/>
+      <c r="F304" t="inlineStr"/>
+      <c r="G304" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H304" t="inlineStr"/>
+      <c r="I304" t="inlineStr"/>
+      <c r="J304" t="inlineStr"/>
+      <c r="K304" t="inlineStr"/>
+      <c r="L304" t="inlineStr"/>
+      <c r="M304" t="inlineStr"/>
+      <c r="N304" t="inlineStr"/>
+      <c r="O304" t="inlineStr"/>
+      <c r="P304" t="inlineStr"/>
+      <c r="Q304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>disrupting-climate-change-futures-conceptual-tools-for-lost-histories</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr"/>
+      <c r="C305" t="inlineStr"/>
+      <c r="D305" t="inlineStr"/>
+      <c r="E305" t="inlineStr"/>
+      <c r="F305" t="inlineStr"/>
+      <c r="G305" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H305" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\disrupting-climate-change-futures-conceptual-tools-for-lost-histories.txt</t>
+        </is>
+      </c>
+      <c r="I305" t="inlineStr"/>
+      <c r="J305" t="inlineStr"/>
+      <c r="K305" t="inlineStr"/>
+      <c r="L305" t="inlineStr"/>
+      <c r="M305" t="inlineStr"/>
+      <c r="N305" t="inlineStr"/>
+      <c r="O305" t="inlineStr"/>
+      <c r="P305" t="inlineStr"/>
+      <c r="Q305" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>social-movements-as-agents-of-change-fighting-intersectional-food-inequalities-building-food-as-webs-of-life</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Social movements as agents of change: Fighting intersectional food inequalities, building food as webs of life</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Motta, Renata</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>Sociological Review</t>
+        </is>
+      </c>
+      <c r="F306" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1177/00380261211009061</t>
+        </is>
+      </c>
+      <c r="G306" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H306" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\social-movements-as-agents-of-change-fighting-intersectional-food-inequalities-building-food-as-webs-of-life.txt</t>
+        </is>
+      </c>
+      <c r="I306" t="inlineStr"/>
+      <c r="J306" t="inlineStr"/>
+      <c r="K306" t="inlineStr"/>
+      <c r="L306" t="inlineStr"/>
+      <c r="M306" t="inlineStr"/>
+      <c r="N306" t="inlineStr">
+        <is>
+          <t>What does the diversity of social movements and food initiatives tell us about processes of social change? I argue that they offer a productive analytical lens to observe social change because they identify injustices and dynamics of inequalities in the food system and are actively engaged in transforming these. Alternative local food initiatives react to the environmental impacts of globalized food relations; food sovereignty movements highlight class inequalities and power asymmetries in the food system that affect people’s rights to culturally appropriate foodways; food justice movements denounce institutional racism; feminist movements fight persistent gender inequalities from food production to consumption; vegan movements defend animal rights. These are often mapped onto different world regions, with food justice movements more present in the US; food sovereignty movements louder in the Global South; feminist food movements more active in Latin America; and local food movements commonly in the Global North. This article brings together diverse strands of activism and research on social inequalities related to food under the conceptual umbrella of food inequalities. In addition to concept building, it contributes to a sociology of food studies by mapping the geopolitics of knowledge about social change behind the growing mobilization around food issues. © The Author(s) 2021.</t>
+        </is>
+      </c>
+      <c r="O306" t="inlineStr"/>
+      <c r="P306" t="inlineStr"/>
+      <c r="Q306" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>Developmental-history-of-soil-concepts-from-a-scientific-perspective</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Developmental history of soil concepts from a scientific perspective</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Mizuta, Katsutoshi; Grunwald, Sabine; Cropper, Wendell P.; Bacon, Allan R.</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>Applied Sciences (Switzerland)</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/app11094275</t>
+        </is>
+      </c>
+      <c r="G307" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H307" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Developmental-history-of-soil-concepts-from-a-scientific-perspective.txt</t>
+        </is>
+      </c>
+      <c r="I307" t="inlineStr"/>
+      <c r="J307" t="inlineStr"/>
+      <c r="K307" t="inlineStr"/>
+      <c r="L307" t="inlineStr"/>
+      <c r="M307" t="inlineStr"/>
+      <c r="N307" t="inlineStr">
+        <is>
+          <t>Various soil concepts have emerged since the beginning of the twentieth century, with some shared similarities. These concepts have contributed to a rise in the awareness of protecting limited soil resources, but not every idea has equally gained widespread attention from scientists. The purpose of this study was to document the developmental history of 10 soil concepts from 1900 to 2018 and investigate their growth/decline. Articles containing words related to the selected soil concepts in titles, abstracts, or publication contents available in the Web of Science were examined. “Soil production” was the oldest concept, found in a paper published in 1910, followed chronologically in the literature by soil care, fertility, conservation, quality, health, protection, security, sustainability, and resilience. Most of the concepts were initially found in non-soil-science journals that predated publications in soil science journals, which implies slowness of the soil science community’s adoption. The statistical publication trend for each concept over time was analyzed and interpreted based on diffusion of innovation theory. The results suggest that all of the soil concepts experienced a statistically positive/upward shift (p &lt; 0.01) over time. In particular, soil concepts cited in soil science journals tended to maintain their momentum and communal value over time in soil science research, except the soil care concept. Applications of soil concept research based on collaboration between scientists of different nationalities, affiliations, and research expertise would further increase the possibility of citation frequency and foster interdisciplinary and transdisciplinary collaboration. © 2021 by the authors. Licensee MDPI, Basel, Switzerland.</t>
+        </is>
+      </c>
+      <c r="O307" t="inlineStr"/>
+      <c r="P307" t="inlineStr"/>
+      <c r="Q307" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>Developing-earthly-attachments-in-the-anthropocene</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Developing earthly attachments in the anthropocene</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Huijbens, Edward H.</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr">
+        <is>
+          <t>Developing Earthly Attachments in the Anthropocene</t>
+        </is>
+      </c>
+      <c r="F308" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.4324/9781003098782</t>
+        </is>
+      </c>
+      <c r="G308" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H308" t="inlineStr"/>
+      <c r="I308" t="inlineStr"/>
+      <c r="J308" t="inlineStr"/>
+      <c r="K308" t="inlineStr"/>
+      <c r="L308" t="inlineStr"/>
+      <c r="M308" t="inlineStr"/>
+      <c r="N308" t="inlineStr">
+        <is>
+          <t>This book explores the development and significance of an Earth-oriented progressive approach to fostering global wellbeing and inclusive societies in an era of climate change and uncertainty. Developing Earthly Attachments in the Anthropocene examines the ways in which the Earth has become a source of political, social, and cultural theory in times of global climate change. The book explains how the Earth contributes to the creation of a regenerative culture, drawing examples from the Netherlands and Iceland. These examples offer understandings of how legacies of non-respectful exploitative practices culminating in the rapid post-war growth of global consumption have resulted in impacts on the ecosystem, highlighting the challenges of living with planet Earth. The book familiarizes readers with the implied agencies of the Earth which become evident in our reliance on the carbon economy - a factor of modern-day globalized capitalism responsible for global environmental change and emergency. It also suggests ways to inspire and develop new ways of spatial sense making for those seeking earthly attachments. Offering novel theoretical and practical insights for politically active people, this book will appeal to those involved in local and national policy making processes. It will also be of interest to academics and students of geography, political science, and environmental sciences. © 2021 Edward H. Huijbens.</t>
+        </is>
+      </c>
+      <c r="O308" t="inlineStr"/>
+      <c r="P308" t="inlineStr"/>
+      <c r="Q308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Sharing-the-harvest-Transformative-artful-and-activist-methodologies-for-urban-agroecology</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr"/>
+      <c r="C309" t="inlineStr"/>
+      <c r="D309" t="inlineStr"/>
+      <c r="E309" t="inlineStr"/>
+      <c r="F309" t="inlineStr"/>
+      <c r="G309" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H309" t="inlineStr"/>
+      <c r="I309" t="inlineStr"/>
+      <c r="J309" t="inlineStr"/>
+      <c r="K309" t="inlineStr"/>
+      <c r="L309" t="inlineStr"/>
+      <c r="M309" t="inlineStr"/>
+      <c r="N309" t="inlineStr"/>
+      <c r="O309" t="inlineStr"/>
+      <c r="P309" t="inlineStr"/>
+      <c r="Q309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>Writing-with-rocks</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Writing with rocks</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>Valtonen, Anu; Pullen, Alison</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr">
+        <is>
+          <t>Gender, Work and Organization</t>
+        </is>
+      </c>
+      <c r="F310" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1111/gwao.12579</t>
+        </is>
+      </c>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H310" t="inlineStr"/>
+      <c r="I310" t="inlineStr"/>
+      <c r="J310" t="inlineStr"/>
+      <c r="K310" t="inlineStr"/>
+      <c r="L310" t="inlineStr"/>
+      <c r="M310" t="inlineStr">
+        <is>
+          <t>Arctic; Australia; Finland; New South Wales; Sydney [New South Wales]; Macropodidae; ethics; feminism; geology; politics; rock</t>
+        </is>
+      </c>
+      <c r="N310" t="inlineStr">
+        <is>
+          <t>Rocks. Geological forces across time and space. Non-human beings. Humans. Affect material encounters with rocks. Connecting. Being. Writing… From the Artic to Eastern Finland. From Sydney to Kangaroo Island, Australia. From the north to the south, and back again. Corporeal, affective. These rocks live with and through us. Touching rocks—rocks touch us. Bodies—rocks, co-constituted in life. Disrupting. Non-violent. Ethico-political acts of writing. Writing rocks. Humans become geologic forces. Care. Response-able. © 2021 John Wiley &amp; Sons Ltd.</t>
+        </is>
+      </c>
+      <c r="O310" t="inlineStr"/>
+      <c r="P310" t="inlineStr"/>
+      <c r="Q310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>Becoming-alive-within-science-education-research</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr"/>
+      <c r="C311" t="inlineStr"/>
+      <c r="D311" t="inlineStr"/>
+      <c r="E311" t="inlineStr"/>
+      <c r="F311" t="inlineStr"/>
+      <c r="G311" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H311" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Becoming-alive-within-science-education-research.txt</t>
+        </is>
+      </c>
+      <c r="I311" t="inlineStr"/>
+      <c r="J311" t="inlineStr"/>
+      <c r="K311" t="inlineStr"/>
+      <c r="L311" t="inlineStr"/>
+      <c r="M311" t="inlineStr"/>
+      <c r="N311" t="inlineStr"/>
+      <c r="O311" t="inlineStr"/>
+      <c r="P311" t="inlineStr"/>
+      <c r="Q311" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>Soil-health-and-well-being-Redefining-soil-health-based-upon-a-plurality-of-values</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Soil health and well-being: Redefining soil health based upon a plurality of values</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>Friedrichsen, Claire N.; Hagen-Zakarison, Sheryl; Friesen, Maren L.; McFarland, Carol R.; Tao, Haiying; Wulfhorst, J.D.</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E312" t="inlineStr">
+        <is>
+          <t>Soil Security</t>
+        </is>
+      </c>
+      <c r="F312" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.soisec.2021.100004</t>
+        </is>
+      </c>
+      <c r="G312" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H312" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Soil-health-and-well-being-Redefining-soil-health-based-upon-a-plurality-of-values.txt</t>
+        </is>
+      </c>
+      <c r="I312" t="inlineStr"/>
+      <c r="J312" t="inlineStr"/>
+      <c r="K312" t="inlineStr"/>
+      <c r="L312" t="inlineStr"/>
+      <c r="M312" t="inlineStr"/>
+      <c r="N312" t="inlineStr">
+        <is>
+          <t>The dominant research paradigm for soil health emphasizes instrumental values to achieve sustainable food systems. However, soil provides a plurality of values in society beyond instrumental value contributing to human well-being. This research aims to understand the relational values that soil provides farmers by examining the meaningfulness and intrinsic motivation for building soil health among wheat farmers in the Inland Pacific Northwest (iPNW). Data were collected from two soil health work sessions and 11 in-depth semi-structured interviews with innovator wheat farmers to understanding broader perspectives and meanings of soil health. Four themes of relational values emerged from the data showing the link between soil health and human well-being. The results suggest that the term soil health should not be exclusively assessed by its instrumental values but also by its relational values supporting a plural valuation of soil health. Incorporating soil health's plural valuation into research will contribute to more effective holistic innovations supporting human and environmental well-being. This research provides important insights into defining soil health and for transforming the innovation paradigm of soil health to include relational values and cultural ecosystem services for transforming our current food system into an equitable, sustainable, healthy, and just system. Changing soil health assessments to acknowledge additional soil health management outcomes related to human well-being may facilitate decision-making, support the intrinsic motivation of soil health, and provide support to transformative food systems. © 2021</t>
+        </is>
+      </c>
+      <c r="O312" t="inlineStr"/>
+      <c r="P312" t="inlineStr"/>
+      <c r="Q312" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>Rupturing-violent-land-imaginaries</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Rupturing violent land imaginaries: finding hope through a land titling campaign in Cambodia</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Schoenberger, Laura; Beban, Alice</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr">
+        <is>
+          <t>Agriculture and Human Values</t>
+        </is>
+      </c>
+      <c r="F313" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1007/s10460-020-10156-z</t>
+        </is>
+      </c>
+      <c r="G313" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H313" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Rupturing-violent-land-imaginaries.txt</t>
+        </is>
+      </c>
+      <c r="I313" t="inlineStr"/>
+      <c r="J313" t="inlineStr"/>
+      <c r="K313" t="inlineStr"/>
+      <c r="L313" t="inlineStr"/>
+      <c r="M313" t="inlineStr"/>
+      <c r="N313" t="inlineStr">
+        <is>
+          <t>In areas of land conflict, fear and the threat of violence work to reproduce imaginaries of land as a resource that powerful people can grab. An urgent question for agrarian scholars and activists is how people can overcome fear so that alternative imaginaries might flourish. In this article, we argue for attention to the affective dimension of imaginaries; ideas of what land is and should be are co-constituted through the material and social, imbued with powerful emotions that enable imaginaries to be reproduced, to be challenged, and even to be transformed. We draw from long-term research projects in Cambodia—a country known for plantation-fuelled dispossession—where the Prime Minister’s surprise announcement of a land titling campaign in 2012 ruptured the wave of land grabbing, creating openings to imagine different outcomes that are rooted in the potential for legal recognition of smallholder claims. Although the campaign was an uncertain rupture in land imaginaries, these moments matter. Land claimants sought to create affective ties with volunteer land surveyors that embedded hopeful land imaginaries in rural areas and into the national cadastral system. The land title in this context is the material bearer of a land imaginary that centres on rural people’s connection to the land, and also reinforces rural people’s connection to the Cambodian state and the potential to gain the state’s protection. We contribute to an emerging literature that locates the formative effects of hope as an orientation and as a method by exploring the possibilities inherent in rupture. © 2020, Springer Nature B.V.</t>
+        </is>
+      </c>
+      <c r="O313" t="inlineStr"/>
+      <c r="P313" t="inlineStr"/>
+      <c r="Q313" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>Nuclear-waste-as-toxic-legacy-and-future-fantasy</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Nuclear waste as toxic legacy and future fantasy</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>Kasperski, Tatiana; Storm, Anna</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr">
+        <is>
+          <t>Geschichte und Gesellschaft</t>
+        </is>
+      </c>
+      <c r="F314" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.13109/GEGE.2020.46.4.682</t>
+        </is>
+      </c>
+      <c r="G314" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H314" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Nuclear-waste-as-toxic-legacy-and-future-fantasy.txt</t>
+        </is>
+      </c>
+      <c r="I314" t="inlineStr"/>
+      <c r="J314" t="inlineStr"/>
+      <c r="K314" t="inlineStr"/>
+      <c r="L314" t="inlineStr"/>
+      <c r="M314" t="inlineStr"/>
+      <c r="N314" t="inlineStr">
+        <is>
+          <t>In this article, we examine how human interactions with nuclear waste, with special regard to responsibilities and temporalities, have changed over time. Based primarily on historical and contemporary accounts, including interviews, we trace the history of how radioactive residue has been conceptualized and handled in Soviet and post-Soviet Russia and Sweden, from the Second World War to the present. By juxtaposing the practices and perspectives of dumping, management and care, our aim is to contribute to current efforts to make sense of waste in the Anthropocene. We conclude that to acknowledge a need for eternal care is to accentuate the interdependence of historical and geological temporalities. © 2021 Vandenhoeck and Ruprecht GmbH and Co. KG. All rights reserved.</t>
+        </is>
+      </c>
+      <c r="O314" t="inlineStr"/>
+      <c r="P314" t="inlineStr"/>
+      <c r="Q314" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>Introduction-to-symposium-Reimagining-land-materiality-affect-tand-the-uneven-trajectories-of-land-transformation</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Introduction to symposium ‘Reimagining land: materiality, affect and the uneven trajectories of land transformation’</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>Sippel, Sarah Ruth; Visser, Oane</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr">
+        <is>
+          <t>Agriculture and Human Values</t>
+        </is>
+      </c>
+      <c r="F315" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1007/s10460-020-10152-3</t>
+        </is>
+      </c>
+      <c r="G315" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H315" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Introduction-to-symposium-Reimagining-land-materiality-affect-tand-the-uneven-trajectories-of-land-transformation.txt</t>
+        </is>
+      </c>
+      <c r="I315" t="inlineStr"/>
+      <c r="J315" t="inlineStr"/>
+      <c r="K315" t="inlineStr"/>
+      <c r="L315" t="inlineStr"/>
+      <c r="M315" t="inlineStr"/>
+      <c r="N315" t="inlineStr">
+        <is>
+          <t>Over the past decade land has again moved to the centre of resource conflicts, agrarian struggles, and competing visions over the future of food and farming. This renewed interest in land necessitates asking the seemingly simple, but pertinent, question ‘what is land?’ To reach a more profound understanding of the uniqueness of land, and what distinguishes land from other resources, this symposium suggests the notion of ‘land imaginaries’ as a crucial lens in the study of current land transformations. Political-economy, and the particular economic, financial, or political interests of various actors involved in land projects do not directly result in, or translate into, outcomes, such as dispossession and enclosure, increased commodification, financialization, and assetization, or mobilization and resistance. All these processes are informed by different imaginaries of land—the underlying understandings, views, and visions of what land is, can, and should be—and associated visions, hopes, and dreams regarding land. Drawing on a variety of case studies from across the world, crossing Global North/South and East/West, and including contemporary and historical instances of land transformation, this symposium addresses the multifaceted ways in which implicit, explicit, and emergent understandings of land shape current land transformations. © 2020, The Author(s).</t>
+        </is>
+      </c>
+      <c r="O315" t="inlineStr"/>
+      <c r="P315" t="inlineStr"/>
+      <c r="Q315" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>Decaying-Words-The-Metaphor-of-Evolution-in-Language-Becomes-Literal-in-a-Canadian-Forest</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Decaying Words: The Metaphor of Evolution in Language Becomes Literal in a Canadian Forest</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Wilson, Joseph</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr">
+        <is>
+          <t>Technology and Language</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.48417/technolang.2021.01.03</t>
+        </is>
+      </c>
+      <c r="G316" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H316" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Decaying-Words-The-Metaphor-of-Evolution-in-Language-Becomes-Literal-in-a-Canadian-Forest.txt</t>
+        </is>
+      </c>
+      <c r="I316" t="inlineStr"/>
+      <c r="J316" t="inlineStr"/>
+      <c r="K316" t="inlineStr"/>
+      <c r="L316" t="inlineStr"/>
+      <c r="M316" t="inlineStr"/>
+      <c r="N316" t="inlineStr">
+        <is>
+          <t>In 2009, two Canadian poets Stephen Collis and Jordan Scott travelled to five different ecosystems within the borders of British Columbia (BC). At each location, they left a copy of the canonical text of physical anthropology, Darwin’s Origin of Species (1859), open to the elements, for one calendar year. The project, documented in the photographic book Decomp turned the poets’ usual mode of expression on its head: instead of manipulating words to create a final work of linguistic expression, the poets let nature dissolve the integrity of the book, leaving words and morphemes dangling in poetic fragments. The Decomp project allows us to reflect on the environmental influences on language, and the organic structure of language. The dominant metaphors that describe language come from the biological world, and from Darwin’s theory of evolution in particular. Languages can be said to evolve, mutate, grow, stagnate and even die. Like the words in Darwin’s text left to the elements, languages can be isolated by geographic factors and left to fossilize without continued exchange with other cultures. In the forests B.C. the metaphorical mapping between biology and language becomes literal. We bear witness to the effects of entropy on the book and as the line between animate and inanimate agents blurs. As the poets piece together the fragments of Darwin’s prose in Decomp, we are confronted with such questions, confronted with the ephemeral nature of language and the acts of assembly we all perform every day in the face of linguistic change, and often, decay. © 2021, St. Petersburg Polytechnic University of Peter the Great. All rights reserved.</t>
+        </is>
+      </c>
+      <c r="O316" t="inlineStr"/>
+      <c r="P316" t="inlineStr"/>
+      <c r="Q316" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>Recipes for Technoutopia</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Recipes for Technoutopia: On hospitality and infrastructure as experimental performance</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>Jordan, Stephanie Beth</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr">
+        <is>
+          <t>Routledge Handbook of Art, Science, and Technology Studies</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.4324/9780429437069-18</t>
+        </is>
+      </c>
+      <c r="G317" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H317" t="inlineStr"/>
+      <c r="I317" t="inlineStr"/>
+      <c r="J317" t="inlineStr"/>
+      <c r="K317" t="inlineStr"/>
+      <c r="L317" t="inlineStr"/>
+      <c r="M317" t="inlineStr"/>
+      <c r="N317" t="inlineStr">
+        <is>
+          <t>Through the performance of a radical brunch, this piece explores questions of inclusion, responsibility, labor, and care in the development of infrastructure, mirroring the many ways in which the promises of big data will solve pressing problems of participation, climate, and culture. By conceiving of infrastructure as experimental performance, I assert that infrastructure is experiential, sensorial, political, and situated. Through the performance, new rich understanding arises that connects infrastructural moments of breakdown, maintenance, and repair to the politics of the personal, orientation, and disorientation, uncovering a dissonance between the rhetoric of future-building and the sociomaterial realities of the present. If the recipe for the future is a technoutopia, this experimental performance asks: what are its ingredients and the labor of its production? Who is the chef, the served, the hungry? What spoils utopias? © 2022 selection and editorial matter, Hannah Star Rogers, Megan K. Halpern, Dehlia Hannah, and Kathryn de Ridder-Vignone individual chapters, the contributors.</t>
+        </is>
+      </c>
+      <c r="O317" t="inlineStr"/>
+      <c r="P317" t="inlineStr"/>
+      <c r="Q317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>Responsible-research-and-innovation-meets-multispecies-studies</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Responsible research and innovation meets multispecies studies: why RRI needs to be a more-than-human exercise</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Szymanski, Erika Amethyst; Smith, Robert D. J.; Calvert, Jane</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr">
+        <is>
+          <t>Journal of Responsible Innovation</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/23299460.2021.1906040</t>
+        </is>
+      </c>
+      <c r="G318" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H318" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Responsible-research-and-innovation-meets-multispecies-studies.txt</t>
+        </is>
+      </c>
+      <c r="I318" t="inlineStr"/>
+      <c r="J318" t="inlineStr"/>
+      <c r="K318" t="inlineStr"/>
+      <c r="L318" t="inlineStr"/>
+      <c r="M318" t="inlineStr"/>
+      <c r="N318" t="inlineStr">
+        <is>
+          <t>We offer an argument for why responsible research and innovation should be in conversation with multispecies studies. We suggest that RRI can learn from multispecies studies to expand definitions of stakeholders and responsibilities, thereby including other creatures in conversations and frameworks where they are currently missing. In addition, the RRI community might benefit from exploring conceptual overlaps between RRI and multispecies studies literatures. For example, concepts germane to RRI–notably, care and relationality–have been particularly well-developed with respect to how they oblige mutually responsive relationships. Consequently, connecting these two areas of theory and practice should nuance discussions about responsibility as an individual versus a collective endeavor and about the relationship between RRI and knowledge production. © 2021 The Author(s). Published by Informa UK Limited, trading as Taylor &amp; Francis Group.</t>
+        </is>
+      </c>
+      <c r="O318" t="inlineStr"/>
+      <c r="P318" t="inlineStr"/>
+      <c r="Q318" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>Glyphosate-A-love-story</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Glyphosate—A love story. Ordinary thoughtlessness and response-ability in industrial farming</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>Müller, Birgit</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>Journal of Agrarian Change</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1111/joac.12374</t>
+        </is>
+      </c>
+      <c r="G319" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H319" t="inlineStr"/>
+      <c r="I319" t="inlineStr"/>
+      <c r="J319" t="inlineStr"/>
+      <c r="K319" t="inlineStr"/>
+      <c r="L319" t="inlineStr"/>
+      <c r="M319" t="inlineStr"/>
+      <c r="N319" t="inlineStr">
+        <is>
+          <t>More than 8.6 billion kilograms of glyphosate have been used worldwide since the 1970s. Herbicide tolerant crops became the lynchpin of the technological revolution for large-scale farming first in the United States and Canada, and now in Europe. Zero-till farming, as a production scheme and a world view, is based on simplifications promoted by a handful of transnational corporations with the complicity of politicians looking for easy solutions for problems, such as climate change, erosion and the hunger in the world. At the same time, the massive use of glyphosate is branded as an endocrine disrupter, causing cancer, male sterility and infertility. It interferes with soil bacteria and acts on the equilibrium of soil fungi. Glyphosate resistant crops connect farmers to far away consumers ingesting the food they grow together with the traces of chemicals. Farmers intra-act with the myriads of life-forms of the soil eco-system. How do they perceive the life in the soil, when they spray chemicals? The article explores the political dimensions of the agency of both humans and non-humans to understand the effects of the modernizing project of zero-till, as well as to identify spaces and scales of possibility from where alternatives can emerge. © 2020 John Wiley &amp; Sons Ltd</t>
+        </is>
+      </c>
+      <c r="O319" t="inlineStr"/>
+      <c r="P319" t="inlineStr"/>
+      <c r="Q319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>Scaffolding-transitions-of-possibility-the-food-walk-as-embodied-method-in-Singapore</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Scaffolding transitions of possibility: the food walk as embodied method in Singapore</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>Ng, Huiying</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr">
+        <is>
+          <t>Journal of Urbanism</t>
+        </is>
+      </c>
+      <c r="F320" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/17549175.2021.1941203</t>
+        </is>
+      </c>
+      <c r="G320" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H320" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Scaffolding-transitions-of-possibility-the-food-walk-as-embodied-method-in-Singapore.txt</t>
+        </is>
+      </c>
+      <c r="I320" t="inlineStr"/>
+      <c r="J320" t="inlineStr"/>
+      <c r="K320" t="inlineStr"/>
+      <c r="L320" t="inlineStr"/>
+      <c r="M320" t="inlineStr"/>
+      <c r="N320" t="inlineStr">
+        <is>
+          <t>Resilient food infrastructures responsive to instability and change often form at the urban edge of food systems. As such, they could take heed of knowledge practices that occur at the urban edge. This paper conceptualizes learning as a co-productive activity that can be scaffolded by space, and examines how it applies to the re-imagination of food systems. By considering walking as a method in the design of desired foodscapes, this paper addresses how “time niches” foster embodied knowledges of care and haptic connection. The two cases that illustrate this–a set of walking workshops with Singapore-based participants and a visualising workshop with visiting conference participants–consider how so-called lay and expert knowledges may come together in knowledge co-production in future-making practices. The paper explores how civic and decolonial practices occur in the sustainability transition of food. © 2021 Informa UK Limited, trading as Taylor &amp; Francis Group.</t>
+        </is>
+      </c>
+      <c r="O320" t="inlineStr"/>
+      <c r="P320" t="inlineStr"/>
+      <c r="Q320" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>Alter-transitional-justice-transforming-unjust-relations-with-the-more-than-human</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Alter-transitional justice; transforming unjust relations with the more-than-human</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>Celermajer, Danielle; O’Brien, Anne Therese</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr">
+        <is>
+          <t>Posthuman Legalities:New Materialism and Law Beyond the Human</t>
+        </is>
+      </c>
+      <c r="F321" t="inlineStr">
+        <is>
+          <t>https://www.scopus.com/inward/record.uri?eid=2-s2.0-85130198688&amp;partnerID=40&amp;md5=7cf71b0b5c8ca61d8ec86558071791a1</t>
+        </is>
+      </c>
+      <c r="G321" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H321" t="inlineStr"/>
+      <c r="I321" t="inlineStr"/>
+      <c r="J321" t="inlineStr"/>
+      <c r="K321" t="inlineStr"/>
+      <c r="L321" t="inlineStr"/>
+      <c r="M321" t="inlineStr"/>
+      <c r="N321" t="inlineStr">
+        <is>
+          <t>Drawing on the emerging field of multispecies justice, this article seeks to understand how the idea of transitional justice, capaciously understood, might be put to work to transform unjust relations between humans and the more-than-human. Reflecting onconcerns in the literatures on animals and the environment concerning the cogency of addressing past wrongs against the more-than-human by using a justice framework, the article sets out a foundational agenda for transitional justice and a conceptual framework responsive to the ontological diversity of beings and communities other than humans. Focusing on soil specifically, the article explores the problem of developing transitional justice approaches for transforming relations that involve systemic violence where such violence is not acknowledged because the harmed being - soil - is not recognized as the type of community to which justice might be owed. To illustrate prototransitional justice, the article considers both the work of regenerative farmers and emergent collaborations between farmers and visual artists to explore how engagements with the arts of relating to the more than-human might move the as yet private transformations of relations with soil into a more public, albeit incipient, process of justice. © Edward Elgar Publishing 2021.</t>
+        </is>
+      </c>
+      <c r="O321" t="inlineStr"/>
+      <c r="P321" t="inlineStr"/>
+      <c r="Q321" t="inlineStr"/>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>Animality-coloniality-COVID-19-and-the-Animal-question</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Animality/coloniality: COVID-19 and the Animal question</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>Isaacs, Jenny R.; Otruba, Ariel</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr">
+        <is>
+          <t>A Research Agenda for Animal Geographies</t>
+        </is>
+      </c>
+      <c r="F322" t="inlineStr">
+        <is>
+          <t>https://www.scopus.com/inward/record.uri?eid=2-s2.0-85123422033&amp;partnerID=40&amp;md5=02fd034bd658a93ea6fea7cfba6a9d2a</t>
+        </is>
+      </c>
+      <c r="G322" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H322" t="inlineStr"/>
+      <c r="I322" t="inlineStr"/>
+      <c r="J322" t="inlineStr"/>
+      <c r="K322" t="inlineStr"/>
+      <c r="L322" t="inlineStr"/>
+      <c r="M322" t="inlineStr"/>
+      <c r="N322" t="inlineStr">
+        <is>
+          <t>Joining efforts to “decolonize geography”, we offer ‘animality/coloniality’ as a heuristic device for analyzing asymmetrical power relations between humans and nonhumanity. The case of COVID-19 is used to demonstrate the complexity, problems, and dangers of defining and deploying the category of ‘animal’. By illustrating how competing ideas of animality are worked through each other in understandings of and responses to zoonotic viruses, we suggest that delinking animality/coloniality should begin with an embrace of the ‘alien’ Other as a pathogenic constituency. While the perennial Animal question remains an important driver of new research in animal geographies, we caution that it should be taken up with reflexive, critical attention to one’s political purpose and situated location within (colonial) knowledge production. © Alice Hovorka, Sandra McCubbin and Lauren Van Patter 2021.</t>
+        </is>
+      </c>
+      <c r="O322" t="inlineStr"/>
+      <c r="P322" t="inlineStr"/>
+      <c r="Q322" t="inlineStr"/>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>PLANTS-PATHOGENS-AND-THE-POLITICS-OF-CARE</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>PLANTS, PATHOGENS, AND THE POLITICS OF CARE: Xylella fastidiosa and the Intra‐active Breakdown of Mallorca's Almond Ecology</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>REISMAN, EMILY</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>Cultural Anthropology</t>
+        </is>
+      </c>
+      <c r="F323" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.14506/ca36.3.07</t>
+        </is>
+      </c>
+      <c r="G323" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H323" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\PLANTS-PATHOGENS-AND-THE-POLITICS-OF-CARE.txt</t>
+        </is>
+      </c>
+      <c r="I323" t="inlineStr"/>
+      <c r="J323" t="inlineStr"/>
+      <c r="K323" t="inlineStr"/>
+      <c r="L323" t="inlineStr"/>
+      <c r="M323" t="inlineStr"/>
+      <c r="N323" t="inlineStr">
+        <is>
+          <t>Almonds were once “the gold of Mallorca,” a source of modest wealth and a pillar of diversified farming systems for smallholders on the largest of Spain's Balearic Islands. Now researchers believe nearly every rainfed almond tree on the island will be dead within as few as five years. The introduced bacteria Xylella fastidiosa, enabled by its spittle‐bug vector, and emboldened by climate change, has flooded the xylem of these rainfed trees, impeding the flow of fluid and nutrients to the point where the tree can no longer survive. This article enrolls feminist theorizations of care and agential realism to broaden the political scope and stakes of a plant epidemic. I argue that by attending to the care relations underlying pathogenicity we can shift from narratives of landscape purification toward a more‐than‐human politics of care. © 2021. All rights reserved.</t>
+        </is>
+      </c>
+      <c r="O323" t="inlineStr"/>
+      <c r="P323" t="inlineStr"/>
+      <c r="Q323" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>Ecological-Transition-What-It-Is-and-How-to-Do-It</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Ecological Transition: What It Is and How to Do It</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>Ghelfi, Andrea; Papadopoulos, Dimitris</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>Tecnoscienza</t>
+        </is>
+      </c>
+      <c r="F324" t="inlineStr">
+        <is>
+          <t>https://www.scopus.com/inward/record.uri?eid=2-s2.0-85130158731&amp;partnerID=40&amp;md5=59a86ecab841037b443a065dc2d0c911</t>
+        </is>
+      </c>
+      <c r="G324" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H324" t="inlineStr"/>
+      <c r="I324" t="inlineStr"/>
+      <c r="J324" t="inlineStr"/>
+      <c r="K324" t="inlineStr"/>
+      <c r="L324" t="inlineStr"/>
+      <c r="M324" t="inlineStr"/>
+      <c r="N324" t="inlineStr">
+        <is>
+          <t>The paper examines different practices, imaginaries and programs of ecological transitions whose articulation points towards a more-than-local and less-than-global green eco-social transformation. Translocal ecological transitions bring together climate action politics, environmental justice, and the everyday ecologism of experimental community-led technoscience. Within transition projects we see the emergence of new more-than-human political constituencies, the making of broad eco-social coalitions, and the implementation of innovative forms of reparative governance. Ecological transitions foster a new political space, green democracy, as an alternative to both regressive nationalism and green globalism that dominate contemporary politics. © 2021 STS Italia. All Rights Reserved.</t>
+        </is>
+      </c>
+      <c r="O324" t="inlineStr"/>
+      <c r="P324" t="inlineStr"/>
+      <c r="Q324" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Nova atualização de bibliografia
</commit_message>
<xml_diff>
--- a/Ontologia de Solos/Pesquisa SCOPUS/Pesquisa_Ontologia_Solos.xlsx
+++ b/Ontologia de Solos/Pesquisa SCOPUS/Pesquisa_Ontologia_Solos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q324"/>
+  <dimension ref="A1:Q344"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22252,6 +22252,1126 @@
       <c r="P324" t="inlineStr"/>
       <c r="Q324" t="inlineStr"/>
     </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>Care-in-Technology-Volume-7</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Care in Technology: Volume 7</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>Guchet, Xavier</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>Care in Technology: Volume 7</t>
+        </is>
+      </c>
+      <c r="F325" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/9781119821403</t>
+        </is>
+      </c>
+      <c r="G325" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H325" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Care-in-Technology-Volume-7.txt</t>
+        </is>
+      </c>
+      <c r="I325" t="inlineStr"/>
+      <c r="J325" t="inlineStr"/>
+      <c r="K325" t="inlineStr"/>
+      <c r="L325" t="inlineStr"/>
+      <c r="M325" t="inlineStr"/>
+      <c r="N325" t="inlineStr">
+        <is>
+          <t>Today, it is widely recognized that in order to meet environmental challenges, it will not simply be enough to make our lifestyles greener; also critical is putting an end to the modern conception of the human as master and possessor of nature. However, to bear fruit, this change in anthropology must also be accompanied by a revision in our conception of technology. Since the Enlightenment and the development of industrialization, technology no longer seems to be subject to the guiding principles set by the Greeks: prudence and the search for the right measure in all, which leads to the care of beings and the world. Care in Technology analyzes the historical changes that have led technology to become an unthinkable part of care, and care an unthinkable part of technology. It also establishes the conditions for care to once again become a regulatory principle of the activity of engineers who design technology. © ISTE Ltd 2021.</t>
+        </is>
+      </c>
+      <c r="O325" t="inlineStr"/>
+      <c r="P325" t="inlineStr"/>
+      <c r="Q325" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>Urban-Ecosystem-Justice</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Urban Ecosystem Justice: Strategies for Equitable Sustainability and Ecological Literacy in the City</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>Kellogg, Scott</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>Urban Ecosystem Justice: Strategies for Equitable Sustainability and Ecological Literacy in the City</t>
+        </is>
+      </c>
+      <c r="F326" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.4324/9780367858711</t>
+        </is>
+      </c>
+      <c r="G326" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H326" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Urban-Ecosystem-Justice.txt</t>
+        </is>
+      </c>
+      <c r="I326" t="inlineStr"/>
+      <c r="J326" t="inlineStr"/>
+      <c r="K326" t="inlineStr"/>
+      <c r="L326" t="inlineStr"/>
+      <c r="M326" t="inlineStr"/>
+      <c r="N326" t="inlineStr">
+        <is>
+          <t>Merging together the fields of urban ecology, environmental justice, and urban environmental education, Urban Ecosystem Justice promotes building fair, accessible, and mutually beneficial relationships between citizens and the soils, water, atmospheres, and biodiversity in their cities. This book provides a framework for recentering issues of justice and fairness in sustainability discourse while challenging the profound ecological alienation experienced by urban residents. While the urban sustainability movement has had many successes in the past few decades, there remain areas for it to grow. For one, the benefits of sustainability have disproportionately benefited wealthier city residents, with concerns over equity, justice, and social sustainability frequently taking a back seat to economic and environmental considerations. Additionally, many city dwellers remain estranged from and unfamiliar with ecological processes, with urban environments often thought of as existing outside of nature or as hopelessly degraded. Through a citizen-centered lens, the book offers a guide to reconciling these issues by demonstrating how questions of equity, access, and justice apply to the biophysical dimensions of the urban ecosystem: Soil, water, air, waste, and biodiversity. Drawing heavily from the fields of urban ecology, environmental justice, and ecological design, this book lays out a science of cities for people: A pedagogical platform that can be used to promote ecological literacy in underrepresented urban communities through affordable and decentralized means. This book provides both a theoretical and practical field guide to students and researchers of urban sustainability, city planners, architects, policymakers, and activists wishing to develop reciprocal relationships with urban ecologies. © 2022 Scott Kellogg.</t>
+        </is>
+      </c>
+      <c r="O326" t="inlineStr"/>
+      <c r="P326" t="inlineStr"/>
+      <c r="Q326" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>Caring-for-strangers-Alterity-alliances-and-reptile-conservation</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Caring for strangers: Alterity, alliances, and reptile conservation in the “gecko garden refuges” in manapany-les-bains, la réunion</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>Krieg, Lisa Jenny</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>Geographische Zeitschrift</t>
+        </is>
+      </c>
+      <c r="F327" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.25162/gz-2020-0007</t>
+        </is>
+      </c>
+      <c r="G327" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H327" t="inlineStr"/>
+      <c r="I327" t="inlineStr"/>
+      <c r="J327" t="inlineStr"/>
+      <c r="K327" t="inlineStr"/>
+      <c r="L327" t="inlineStr"/>
+      <c r="M327" t="inlineStr">
+        <is>
+          <t>Indian Ocean; Indian Ocean (West); Mascarene Islands; Reunion; ethnography; exploration; mammal; reptile</t>
+        </is>
+      </c>
+      <c r="N327" t="inlineStr">
+        <is>
+          <t>Commonly seen as either dangerous or unsocial, reptiles represent a kind of alterity that is often deemed categorically different from warm-blooded mammals. In the village of Manapany-les-Bains, however, on the island of La Réunion in the Western Indian Ocean, care for the endangered gecko species Phelsuma inexpectata has taken an unexpected turn: initiated by a local NGO, village residents have declared their private gardens a gecko-friendly zone. Engaging concepts of multispecies care and alterity, this article explores what caring for a reptile means. Based on ethnographic field research in Manapany-les-Bains, I will discuss how the gecko's otherness remains an ambivalent trope, being both reduced and capitalized on, and that new alliances are exclusionary and fragmented. © Franz Steiner Verlag, Stuttgart 2020</t>
+        </is>
+      </c>
+      <c r="O327" t="inlineStr"/>
+      <c r="P327" t="inlineStr"/>
+      <c r="Q327" t="inlineStr"/>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>Plastic-pigs-and-public-secrets-in-translational-neonatology-in-Denmark</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Plastic pigs and public secrets in translational neonatology in Denmark</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>Dam, Mie S.; Sangild, Per T.; Svendsen, Mette N.</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>Palgrave Communications</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1057/s41599-020-0463-y</t>
+        </is>
+      </c>
+      <c r="G328" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H328" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Plastic-pigs-and-public-secrets-in-translational-neonatology-in-Denmark.txt</t>
+        </is>
+      </c>
+      <c r="I328" t="inlineStr"/>
+      <c r="J328" t="inlineStr"/>
+      <c r="K328" t="inlineStr"/>
+      <c r="L328" t="inlineStr"/>
+      <c r="M328" t="inlineStr"/>
+      <c r="N328" t="inlineStr">
+        <is>
+          <t>This paper explores how a translational research platform in Denmark uses piglets as infant models. Drawing on meanings of “public” as “open” and “visible,” we track how researchers and clinicians together and separately turn research piglets and premature infants into both public and un-public beings in laboratory and clinical settings. In these complex multispecies relationships, researchers and clinicians alike create and retain certain “zones of unknowing” in which intimate cross-species care relations are fostered. While critical social scientists call for greater public recognition of animals in accounts of human health, our study demonstrates that “zones of unknowing” enable the involved professionals to care simultaneously for neonatal beings and the greater public good. To account for the efforts involved in contributing to the greater public good, we introduce the term “publication work.” We argue that publication work relies as much on porosity between species and spaces as on actively drawing boundaries between species and between public and private spaces. Plastic pigs and public secrets are crucial to realise the ambition of more-than-human public health. © 2020, The Author(s).</t>
+        </is>
+      </c>
+      <c r="O328" t="inlineStr"/>
+      <c r="P328" t="inlineStr"/>
+      <c r="Q328" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>Rhythms-of-Law-Aboriginal-Jurisprudence-and-the-Anthropocene</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Rhythms of Law: Aboriginal Jurisprudence and the Anthropocene</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>Wright, Kate</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>Law and Critique</t>
+        </is>
+      </c>
+      <c r="F329" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1007/s10978-020-09279-3</t>
+        </is>
+      </c>
+      <c r="G329" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H329" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Rhythms-of-Law-Aboriginal-Jurisprudence-and-the-Anthropocene.txt</t>
+        </is>
+      </c>
+      <c r="I329" t="inlineStr"/>
+      <c r="J329" t="inlineStr"/>
+      <c r="K329" t="inlineStr"/>
+      <c r="L329" t="inlineStr"/>
+      <c r="M329" t="inlineStr"/>
+      <c r="N329" t="inlineStr">
+        <is>
+          <t>On 1 December 2019, over one hundred Aboriginal nations performed ancestral and creation dances in synchrony across the Australian continent. One of the communities that danced was the Anaiwan nation from the north-eastern region of New South Wales, Australia. Since 2014 I have been working with Anaiwan people in a collaborative activist research project, creating and maintaining an Aboriginal community garden on the fringes of my hometown of Armidale as a site for land reclamation and decolonising, multispecies research. The community garden is adjacent to the site of the old East Armidale Aboriginal Reserve, where over one hundred dispossessed Aboriginal people were forced to live on the municipal town garbage depot in the mid-twentieth century. This paper positions both the Nation Dance 2019 movement, and the Armidale Aboriginal Community Garden, as rhythmic events that activate Aboriginal Law and sovereignty that is held enduring in the land but that has been buried alive by the settler-colonial state. Focusing on the tensions between deep Indigenous ancestral temporality and colonial territoriality, I argue that the emergence of the Anthropocene reveals a dangerous dissonance between the rhythms of Aboriginal Law patterned through present-day Australian environments and the grid-based structures of colonial governance imposed upon them. © 2020, Springer Nature B.V.</t>
+        </is>
+      </c>
+      <c r="O329" t="inlineStr"/>
+      <c r="P329" t="inlineStr"/>
+      <c r="Q329" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>Organic-taste-and-labour-on-Indian-tea-plantations</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Organic taste and labour on Indian tea plantations*</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>Kumpf, Desirée</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>Social Anthropology</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1111/1469-8676.12951</t>
+        </is>
+      </c>
+      <c r="G330" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H330" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Organic-taste-and-labour-on-Indian-tea-plantations.txt</t>
+        </is>
+      </c>
+      <c r="I330" t="inlineStr"/>
+      <c r="J330" t="inlineStr"/>
+      <c r="K330" t="inlineStr"/>
+      <c r="L330" t="inlineStr"/>
+      <c r="M330" t="inlineStr"/>
+      <c r="N330" t="inlineStr">
+        <is>
+          <t>This paper takes a multispecies perspective on taste to explore how organic agriculture affects both nonhuman relations and human labour on Indian tea plantations. Organic tea planters use taste to assess soil conditions and climatic changes and to apply organic practices accordingly. The paper argues that, on the one hand, planters strategically cultivate forms of collaboration between tea plants, fungi, cows and soil microorganisms to enhance the taste of monoculture crops. On the other hand, since these collaborative forms require and reproduce the precarious labour of tea workers and supervisors, their resistance against organic practices also affects tastes. The terroir of organic tea features both the multispecies ‘togetherness’ on monocultures and the inequalities of plantation labour. © 2020 The Authors. Social Anthropology published by Wiley Periodicals LLC on behalf of European Association of Social Anthropologists.</t>
+        </is>
+      </c>
+      <c r="O330" t="inlineStr"/>
+      <c r="P330" t="inlineStr"/>
+      <c r="Q330" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>Blue-space-as-caring-space-water</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Blue space as caring space–water and the cultivation of care in social and environmental practice; [  L’espace bleu en tant qu’espace de soins–l’eau et la culture de soins dans la pratique sociale et environnementale]; [  El espacio azul como espacio de cuidado — el agua y el cultivo del cuidado en la práctica social y ambiental]</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>Buser, Michael; Payne, Tom; Edizel, Özlem; Dudley, Lyze</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>Social and Cultural Geography</t>
+        </is>
+      </c>
+      <c r="F331" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/14649365.2018.1534263</t>
+        </is>
+      </c>
+      <c r="G331" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H331" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Blue-space-as-caring-space-water.txt</t>
+        </is>
+      </c>
+      <c r="I331" t="inlineStr"/>
+      <c r="J331" t="inlineStr"/>
+      <c r="K331" t="inlineStr"/>
+      <c r="L331" t="inlineStr"/>
+      <c r="M331" t="inlineStr">
+        <is>
+          <t>Bristol [Bristol (ADS)]; Bristol [England]; England; Leeds [England]; London [England]; United Kingdom; environmental change; environmental management; environmentalism; greenspace; social change; water management</t>
+        </is>
+      </c>
+      <c r="N331" t="inlineStr">
+        <is>
+          <t>This paper studies three sites or ‘landscapes of care’ in Leeds, Bristol and London where water and associated built and natural environments are used to co-construct and facilitate forms of social and environmental care. Our research narrates the ways in which blue spaces are cultivated for the production of particular forms of caring bodies and sensibilities. Interpreting care as both a doing (caring for) and emotion (caring about), we draw attention to the diverse practices and distributed nature of care in these environments. Our paper has three main insights. First, we draw attention to the role of water as both a material and site of care. Second, we identify a range of more-than-human benefits associated with blue spaces and how these emerge via collaborative, non-linear and reciprocal forms of care. Third, we argue that by understanding how care works in everyday social practice, new forms of ecological care and pro-environmental ways of living with the world can emerge. © 2018 The Author(s). Published by Informa UK Limited, trading as Taylor &amp; Francis Group.</t>
+        </is>
+      </c>
+      <c r="O331" t="inlineStr"/>
+      <c r="P331" t="inlineStr"/>
+      <c r="Q331" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>Diverging-temporalities-of-care-work-on-urban-farms</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Diverging temporalities of care work on urban farms: Negotiating history, responsibility, and productivity in Lithuania</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>Mincytė, Diana; Bartkienė, Aistė; Bikauskaitė, Renata</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>Geoforum</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.geoforum.2020.06.006</t>
+        </is>
+      </c>
+      <c r="G332" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H332" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Diverging-temporalities-of-care-work-on-urban-farms.txt</t>
+        </is>
+      </c>
+      <c r="I332" t="inlineStr"/>
+      <c r="J332" t="inlineStr"/>
+      <c r="K332" t="inlineStr"/>
+      <c r="L332" t="inlineStr"/>
+      <c r="M332" t="inlineStr">
+        <is>
+          <t>Lithuania; agricultural development; agricultural practice; agricultural production; farming system; spatiotemporal analysis; urban area</t>
+        </is>
+      </c>
+      <c r="N332" t="inlineStr">
+        <is>
+          <t>While scholars have developed a nuanced understanding of agriculture as a form of care, the temporal organization of farming practices has received little consideration. Focusing on how farmers organize and experience agriculture, we track diverging approaches to care work on urban farms in Vilnius, Lithuania. Our ethnographic fieldwork and interviews show how Lithuanian urban farmers are struggling to reconcile the civic ideals of the global urban farming movement with their historical understandings of care for specific plants and the land. Whereas the older generation views farming as kinship-based individualized work focusing on particular plants and garden ecologies, the younger generation approaches it as a way to unwind, mediate, and build a community. These different perspectives on farming translate into divergent temporalities of care in which productivist goals rooted in socialist self-provisioning practices and embodied in orderly landscapes encounter new trends of agricultural care manifested in the natural aesthetics of the farms. We examine dynamic tensions between the two farming modalities by linking them to different understandings of moral commitments and responsibilities for plants and land. Through the lens of temporality, we also show how these divergent care modes are themselves grounded in gender inequalities reproduced on the farms and enabled by by the welfare state institutions, including maternity leave and retirement policies. © 2020 Elsevier Ltd</t>
+        </is>
+      </c>
+      <c r="O332" t="inlineStr"/>
+      <c r="P332" t="inlineStr"/>
+      <c r="Q332" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>The-moral-work-of-timing-mobilities</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>The moral work of timing mobilities: ‘limited insight’ and truncated worth in municipal traffic management</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>Wagenknecht, Susann</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>Mobilities</t>
+        </is>
+      </c>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/17450101.2020.1802105</t>
+        </is>
+      </c>
+      <c r="G333" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H333" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\The-moral-work-of-timing-mobilities.txt</t>
+        </is>
+      </c>
+      <c r="I333" t="inlineStr"/>
+      <c r="J333" t="inlineStr"/>
+      <c r="K333" t="inlineStr"/>
+      <c r="L333" t="inlineStr"/>
+      <c r="M333" t="inlineStr">
+        <is>
+          <t>mobility; morality; public administration; traffic management; transportation infrastructure; urban transport</t>
+        </is>
+      </c>
+      <c r="N333" t="inlineStr">
+        <is>
+          <t>Timing urban traffic is moral work. In this paper, I show how the moral work that goes into timing traffic lights addresses both industrial, civic, and domestic worth in ways that cut generalization short. Relying upon ethnographic fieldwork, this paper focuses on how municipal traffic engineering maintains traffic lights and handles complaints about them. Steeped in moral ambiguity, the paper argues, municipal traffic engineering resorts to singularizing complaints, truncating worth, and working with careful dedication from one contestable compromise to the next. With this argument, the paper contributes to an understanding of the temporal and moral orderings at stake in adjusting and justifying urban mobilities. © 2020 Informa UK Limited, trading as Taylor &amp; Francis Group.</t>
+        </is>
+      </c>
+      <c r="O333" t="inlineStr"/>
+      <c r="P333" t="inlineStr"/>
+      <c r="Q333" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>The-swarming-life-of-pastures</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>The swarming life of pastures: living with vole outbreaks in the French Jura uplands</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>Meulemans, Germain</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>Social Anthropology</t>
+        </is>
+      </c>
+      <c r="F334" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1111/1469-8676.12786</t>
+        </is>
+      </c>
+      <c r="G334" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H334" t="inlineStr"/>
+      <c r="I334" t="inlineStr"/>
+      <c r="J334" t="inlineStr"/>
+      <c r="K334" t="inlineStr"/>
+      <c r="L334" t="inlineStr"/>
+      <c r="M334" t="inlineStr"/>
+      <c r="N334" t="inlineStr">
+        <is>
+          <t>This paper addresses the joint becoming of landscapes, agricultural tasks and prairie rodents in the French Jura uplands, where the development of hay monoculture triggered outbreaks of water voles that reduce pastures to dust. I explore links between processual landscape anthropology and contemporary scholarship on more-than-human entanglements in order to follow how ecological disruptions called for the development of new arts of noticing towards multispecies life. I first describe the relationships between Jura farmers, voles, fields and agricultural modernisation programmes, and suggest that vole outbreaks bring these together around shared tasks. I then consider how disputes over how to control voles led to changes in farmers’ ways of caring for their cows and tending the fields. I argue that these underlined changes in their ways of understanding and responding to the rhythms of the landscape’s more-than-human activities. Finally, I draw on the example of conflicts between farmers over whether cows or pastures should be more central to their work. I make the case that to be attentive to fields as a landscape in the Jura is ultimately to define the (in)appropriateness of certain actions and tasks. It becomes constitutive of what ‘good farming’ should be, and precipitates new identities. © 2020 European Association of Social Anthropologists</t>
+        </is>
+      </c>
+      <c r="O334" t="inlineStr"/>
+      <c r="P334" t="inlineStr"/>
+      <c r="Q334" t="inlineStr"/>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>Political-ecology-of-milk-Contested-futures-of-a-lively-food</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Political ecology of milk: Contested futures of a lively food</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>Clay, Nathan; Yurco, Kayla</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>Geography Compass</t>
+        </is>
+      </c>
+      <c r="F335" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1111/gec3.12497</t>
+        </is>
+      </c>
+      <c r="G335" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H335" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Political-ecology-of-milk-Contested-futures-of-a-lively-food.txt</t>
+        </is>
+      </c>
+      <c r="I335" t="inlineStr"/>
+      <c r="J335" t="inlineStr"/>
+      <c r="K335" t="inlineStr"/>
+      <c r="L335" t="inlineStr"/>
+      <c r="M335" t="inlineStr">
+        <is>
+          <t>agricultural development; agricultural management; agricultural production; dairy farming; environmental politics; food security; future prospect; milk; political economy</t>
+        </is>
+      </c>
+      <c r="N335" t="inlineStr">
+        <is>
+          <t>This article advances thinking on the political ecology of food and agriculture by reviewing research on milk and dairy. As increasingly contested foods, milk and dairy provide a window onto inter-linked social and environmental crises and attempts to solve them through adjustments to food production and consumption. We critically assess three trajectories of change (more milk, better milk, and less milk) that are representative of broader efforts to fix social-environmental crises through food. Arguing that these efforts eschew systemic change, we discuss how ideas from food studies, agrarian political economy, and development studies can be united in a potentially transformative research agenda on the political ecology of milk (as well as other foods). We reflect on how concepts of justice, power, and care might inform a political ecology of food and agriculture that can help envision and enact more democratic food futures. © 2020 The Authors. Geography Compass published by John Wiley &amp; Sons Ltd.</t>
+        </is>
+      </c>
+      <c r="O335" t="inlineStr"/>
+      <c r="P335" t="inlineStr"/>
+      <c r="Q335" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>RRI-s-Commitment-to-Care-and-Vulnerability-of-Agrarian-Systems</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>RRI’s Commitment to Care and Vulnerability of Agrarian Systems: The ‘Problem’ of Rice Straw Burning in India</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>Pandey, Poonam</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>Science, Technology and Society</t>
+        </is>
+      </c>
+      <c r="F336" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1177/0971721820902965</t>
+        </is>
+      </c>
+      <c r="G336" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H336" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\RRI-s-Commitment-to-Care-and-Vulnerability-of-Agrarian-Systems.txt</t>
+        </is>
+      </c>
+      <c r="I336" t="inlineStr"/>
+      <c r="J336" t="inlineStr"/>
+      <c r="K336" t="inlineStr"/>
+      <c r="L336" t="inlineStr"/>
+      <c r="M336" t="inlineStr">
+        <is>
+          <t>India; burning; demand analysis; farming system; rice; straw; vulnerability</t>
+        </is>
+      </c>
+      <c r="N336" t="inlineStr">
+        <is>
+          <t>This paper employs RRI’s mandate of ‘commitment to care’ to understand the ‘problem’ of rice straw burning in India and the possible ways of engaging with it. Straw burning is often framed as a linear technology or policy deficit ‘problem’ in need of an immediate and quick fix. Interventions and solutions emerging from such framings have so far remained ineffective. The ‘commitment to care’ approach enables us to situate the current practices of straw burning in a complex web of relationalities, dependencies, vulnerabilities, and affect. By doing so, the ‘problem’ of straw burning is rearticulated and redefined as a cumulative effect of multiple interventions, transformations, and contradictions that led to the shaping of modern agricultural systems in India. This re-articulation demands for a rethinking of engagement, remedies and responsibilities in ways that move beyond the individualization of blame and action. © 2020 SAGE Publications.</t>
+        </is>
+      </c>
+      <c r="O336" t="inlineStr"/>
+      <c r="P336" t="inlineStr"/>
+      <c r="Q336" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>The-Peasant-Way-of-a-More-than-Radical-Democracy</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr"/>
+      <c r="C337" t="inlineStr"/>
+      <c r="D337" t="inlineStr"/>
+      <c r="E337" t="inlineStr"/>
+      <c r="F337" t="inlineStr"/>
+      <c r="G337" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H337" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\The-Peasant-Way-of-a-More-than-Radical-Democracy.txt</t>
+        </is>
+      </c>
+      <c r="I337" t="inlineStr"/>
+      <c r="J337" t="inlineStr"/>
+      <c r="K337" t="inlineStr"/>
+      <c r="L337" t="inlineStr"/>
+      <c r="M337" t="inlineStr"/>
+      <c r="N337" t="inlineStr"/>
+      <c r="O337" t="inlineStr"/>
+      <c r="P337" t="inlineStr"/>
+      <c r="Q337" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>Plants-Crop-diversity-pre-breeding-technologies</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Plants: Crop diversity pre-breeding technologies as agrarian care co-opted?</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>Graddy-Lovelace, Garrett</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>Area</t>
+        </is>
+      </c>
+      <c r="F338" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1111/area.12499</t>
+        </is>
+      </c>
+      <c r="G338" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H338" t="inlineStr"/>
+      <c r="I338" t="inlineStr"/>
+      <c r="J338" t="inlineStr"/>
+      <c r="K338" t="inlineStr"/>
+      <c r="L338" t="inlineStr"/>
+      <c r="M338" t="inlineStr">
+        <is>
+          <t>agricultural technology; breeding; crop plant; cultivation; farmers knowledge; phenotype; species diversity; technological development</t>
+        </is>
+      </c>
+      <c r="N338" t="inlineStr">
+        <is>
+          <t>Within the realm of international agricultural biodiversity conservation, there has been a surge of funding for “pre-breeding” of plant genetic resources for food and agriculture. Molecular high-throughput analysis, among other techniques, attempts to discern, document, and digitise the genomic traits of farmer/landrace varieties and crop wild relatives stored in gene banks to render them legible fodder for professional breeding. But pre-breeding necessitates thorough phenotypic evaluation and characterisation to understand the physiological attributes, heritable traits, and responses of a plant through its life cycle, under various growing and climactic conditions. This paper explores the irony that a range of surveillance technologies have been developed and deployed to mimic the agrarian work and skills of observing plants and attending to how they are faring, what they like and do not like over many seasons and contexts. These calls and technologies acknowledge the need for heedful attention to crops, even as they further displace actual farmers and their longstanding modes of selecting and saving open-pollinated seeds each harvest. Here, attending to crops entails remembering and communicating collectively gathered information of and from the plant. Such agrarian expertise of caring for plants has been systematically devalued and de-intellectualised, with gendered implications. Drawing on feminist geographies and political ecology, a landscape of care framework discloses the matrix of human and beyond-human care at work in cultivating agricultural biodiversity. Rather than ushering in a new valuation of this expertise, new pre-breeding technologies and trainings continue to ignore on-farm, plant-based care work and the farmers who do it. Calling out this contradiction could help re-centre such agrarian care skills as the crux to effective agricultural biodiversity utilisation. The proliferation of pre-breeding technologies could signify the co-optation of agrarian care skills or the opportunity to re-centre and revalue them. The information, practices and views in this article are those of the author(s) and do not necessarily reflect the opinion of the Royal Geographical Society (with IBG). © 2020 Royal Geographical Society (with the Institute of British Geographers).</t>
+        </is>
+      </c>
+      <c r="O338" t="inlineStr"/>
+      <c r="P338" t="inlineStr"/>
+      <c r="Q338" t="inlineStr"/>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>Accomplishing-an-adaptive-clinical-trial-for-cancer</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Accomplishing an adaptive clinical trial for cancer: Valuation practices and care work across the laboratory and the clinic</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>Swallow, Julia; Kerr, Anne; Chekar, Choon Key; Cunningham-Burley, Sarah</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>Social Science and Medicine</t>
+        </is>
+      </c>
+      <c r="F339" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.socscimed.2020.112949</t>
+        </is>
+      </c>
+      <c r="G339" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H339" t="inlineStr">
+        <is>
+          <t>c:\workspace\artigos\Ontologia de Solos\Pesquisa SCOPUS\Textos_Extraidos\Accomplishing-an-adaptive-clinical-trial-for-cancer.txt</t>
+        </is>
+      </c>
+      <c r="I339" t="inlineStr"/>
+      <c r="J339" t="inlineStr"/>
+      <c r="K339" t="inlineStr"/>
+      <c r="L339" t="inlineStr"/>
+      <c r="M339" t="inlineStr">
+        <is>
+          <t>Adaptive Clinical Trials as Topic; Delivery of Health Care; Female; Humans; Laboratories; Male; Neoplasms; Qualitative Research; United Kingdom; cancer; drug development; drug prescribing; genomics; health care; qualitative analysis; research work; Article; biomedicine; cancer research; clinical laboratory; clinical practice; clinical trial (topic); general practitioner; genome analysis; health care organization; health personnel attitude; human; malignant neoplasm; patient care; qualitative research; tumor biopsy; United Kingdom; adaptive clinical trial (topic); female; health care delivery; laboratory; male; neoplasm</t>
+        </is>
+      </c>
+      <c r="N339" t="inlineStr">
+        <is>
+          <t>A new generation of adaptive, multi-arm clinical trials has been developed in cancer research including those offering experimental treatments to patients based on the genomic analysis of their cancer. Depending on the molecular changes found in patients’ cancer cells, it is anticipated that targeted and personalised therapies will be made available for those who have reached the end of standard treatment options, potentially extending survival time. Results from these trials are also expected to advance genomic knowledge for patients in the future. Drawing on data from a qualitative study of one such trial in the UK, comprising observations of out-patient clinic appointments, out-patient biopsy procedures, laboratory work, and interviews with practitioners, this paper explores how the clinical and research value of one such trial was accomplished in everyday practice by focussing on the work of clinical trials and laboratory staff across recruitment, laboratory analysis, and results management. In the face of numerous potential set-backs, disappointments and failure, we explore how practitioners worked to balance the need to meet established measures of value such as numbers of patients recruited into the trial, alongside cultivating the value of positive affects for patients by managing their expectations and emotions. This care work was performed primarily by practitioners whose roles have historically been devalued in healthcare practice and yet, as we show, were critical to this process. We conclude by arguing that as complex multi-arm adaptive trials become more commonplace, we need to attend to, and render visible, the dynamic and care-full valuation practices of backstage practitioners through which experimental biomedicine is accomplished, and in doing so show that care both achieves clinical and research value, and is also a series of practices and processes that tends to tissue, patients and staff in the context of ever-present possibility of failure. © 2020 The Authors</t>
+        </is>
+      </c>
+      <c r="O339" t="inlineStr"/>
+      <c r="P339" t="inlineStr"/>
+      <c r="Q339" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>Nonhuman-labor-and-the-making-of-resources-making-soil</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Nonhuman labor and the making of resources making soils a resource through microbial labor</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>Krzywoszynska, Anna</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>Environmental Humanities</t>
+        </is>
+      </c>
+      <c r="F340" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1215/22011919-8142319</t>
+        </is>
+      </c>
+      <c r="G340" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H340" t="inlineStr"/>
+      <c r="I340" t="inlineStr"/>
+      <c r="J340" t="inlineStr"/>
+      <c r="K340" t="inlineStr"/>
+      <c r="L340" t="inlineStr"/>
+      <c r="M340" t="inlineStr">
+        <is>
+          <t>agricultural labor; ecological modernization; ethnography; nature-society relations; soil biota; soil improvement</t>
+        </is>
+      </c>
+      <c r="N340" t="inlineStr">
+        <is>
+          <t>With soils increasingly seen as living ecosystems, the understanding of the relationship between soils and agricultural labor is changing. A shift from working the soil to working with the soil is hoped to deliver a true ecological modernization of capitalist agriculture, making the production of ever-growing yields and the maintenance of healthy ecosystems co-constitutive. Drawing on ethnographic data from English farming, this article argues that the current trends are in fact a continuation of the logic of capitalist soil improvement in which soils are made into economic resources. By proposing a new conceptualization of labor as a material process of transformation oriented toward the generation of capital value, the author establishes a dialogue between hitherto separate literatures on the making of economic resources and on nonhuman labor. This approach transforms the debates on the relationship between nature and capital by productively collapsing the distinction between labor and resources. The author argues that acknowledging the material co-constitution of (any form of) labor and resource making allows us to better analyze the processes through which natures are rolled into capital. Today's enrollment of soil biota as labor thus opens up the whole biosphere to the logic of improvement, and to the operations of capital. © 2020 Anna Krzywoszynska.</t>
+        </is>
+      </c>
+      <c r="O340" t="inlineStr"/>
+      <c r="P340" t="inlineStr"/>
+      <c r="Q340" t="inlineStr"/>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>The-science-question-in-alternative-agricultures</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>The science question in alternative agricultures: Zero budget natural farming and the emergence of agronomical pluralism in India</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>Münster, Daniel</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>Science and Scientification in South Asia and Europe</t>
+        </is>
+      </c>
+      <c r="F341" t="inlineStr">
+        <is>
+          <t>https://www.scopus.com/inward/record.uri?eid=2-s2.0-85105196048&amp;partnerID=40&amp;md5=68171b76bfc4371a3b7991ef56178ae5</t>
+        </is>
+      </c>
+      <c r="G341" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H341" t="inlineStr"/>
+      <c r="I341" t="inlineStr"/>
+      <c r="J341" t="inlineStr"/>
+      <c r="K341" t="inlineStr"/>
+      <c r="L341" t="inlineStr"/>
+      <c r="M341" t="inlineStr"/>
+      <c r="N341" t="inlineStr"/>
+      <c r="O341" t="inlineStr"/>
+      <c r="P341" t="inlineStr"/>
+      <c r="Q341" t="inlineStr"/>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>Valuing-plants-in-devalued-space</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Valuing plants in devalued spaces: Caring for Baltimore's Street trees</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>Shcheglovitova, Mariya</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>Environment and Planning E: Nature and Space</t>
+        </is>
+      </c>
+      <c r="F342" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1177/2514848619854375</t>
+        </is>
+      </c>
+      <c r="G342" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H342" t="inlineStr"/>
+      <c r="I342" t="inlineStr"/>
+      <c r="J342" t="inlineStr"/>
+      <c r="K342" t="inlineStr"/>
+      <c r="L342" t="inlineStr"/>
+      <c r="M342" t="inlineStr"/>
+      <c r="N342" t="inlineStr">
+        <is>
+          <t>Baltimore City, MD is addressing its future with expansive sustainability initiatives. These include an aggressive tree planting campaign to double the city's tree canopy by 2037. While discourses of greening present tree plantings and related programs as a resolution for the legacies of racist housing market practices, these programs are themselves subject to the legacies of spatial inequalities in access to infrastructural care. Sustainability discourses present urban trees as inherently valuable economically and environmentally but these discourses are disconnected from trees' needs for ongoing care and maintenance. The daily material practices of caring for and maintaining trees are deprioritized in favor of planting more trees to gain these supposedly “inherent” benefits. In the spaces where trees were meant to bring economic and environmental vitality, their deaths reinforce the racist legacies they claim to correct. This paper examines these links and contradictions within the framework of relational urban political ecology. Through a lens of care, this paper shows how humans and non/humans actively co-construct urban space and how just spaces can come about through attention to the needs of humans and non/humans. © The Author(s) 2019.</t>
+        </is>
+      </c>
+      <c r="O342" t="inlineStr"/>
+      <c r="P342" t="inlineStr"/>
+      <c r="Q342" t="inlineStr"/>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>Mountain-Bike-Trail-Building-Dirty-Work-and-a New-Terrestrial-Politics</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Mountain Bike Trail Building, “Dirty” Work, and a New Terrestrial Politics</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>Cherrington, Jim; Black, Jack</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>World Futures</t>
+        </is>
+      </c>
+      <c r="F343" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1080/02604027.2019.1698234</t>
+        </is>
+      </c>
+      <c r="G343" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H343" t="inlineStr"/>
+      <c r="I343" t="inlineStr"/>
+      <c r="J343" t="inlineStr"/>
+      <c r="K343" t="inlineStr"/>
+      <c r="L343" t="inlineStr"/>
+      <c r="M343" t="inlineStr"/>
+      <c r="N343" t="inlineStr">
+        <is>
+          <t>Dirt is evoked to signify many important facets of mountain bike culture, including its emergence, history, and everyday forms of practice and affect. These significations are also drawn on to frame the sport's (sub)cultural and counterideological affiliations. In this article we examine how both the practice of mountain biking and, specifically, mountain bike trail building, raises questions over the object and latent function of dirt, hinting at the way that abjection can, under certain circumstances, be a source of intrigue and pleasure. In doing so, we suggest a resymbolization of our relationship with dirt via a consideration of the terrestrial. © 2019, © 2019 Taylor &amp; Francis Group, LLC.</t>
+        </is>
+      </c>
+      <c r="O343" t="inlineStr"/>
+      <c r="P343" t="inlineStr"/>
+      <c r="Q343" t="inlineStr"/>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>Geophagiac-Art-Food-Dirt</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Geophagiac: Art, Food, Dirt</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>Kelley, Lindsay</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>Thinking with Soils: Material Politics and Social Theory</t>
+        </is>
+      </c>
+      <c r="F344" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.5040/9781350109568.ch-012</t>
+        </is>
+      </c>
+      <c r="G344" t="inlineStr">
+        <is>
+          <t>snowballing Making-time-for-soil</t>
+        </is>
+      </c>
+      <c r="H344" t="inlineStr"/>
+      <c r="I344" t="inlineStr"/>
+      <c r="J344" t="inlineStr"/>
+      <c r="K344" t="inlineStr"/>
+      <c r="L344" t="inlineStr"/>
+      <c r="M344" t="inlineStr"/>
+      <c r="N344" t="inlineStr"/>
+      <c r="O344" t="inlineStr"/>
+      <c r="P344" t="inlineStr"/>
+      <c r="Q344" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>